<commit_message>
minor changes to docs
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todds\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:40009_{CD32B16C-7DED-40CD-BACE-1126F2EAFF7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FEBDF5E5-E94B-4EC0-AA2B-D98D82A82A51}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:40009_{CD32B16C-7DED-40CD-BACE-1126F2EAFF7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A2EABAD4-1F11-4F53-A128-8669F7CACB79}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14712" windowHeight="8808" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="8805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="69">
   <si>
     <t>ModelType</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>SDE</t>
+  </si>
+  <si>
+    <t>* All comtaminated signals have signal-to-noise of 6 dB</t>
   </si>
 </sst>
 </file>
@@ -1093,14 +1096,14 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1216,10 +1219,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>782.77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1299,10 +1302,10 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1370,10 +1373,10 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>0.61899999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1475,7 +1478,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1526,10 +1529,10 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1631,7 +1634,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1745,10 +1748,10 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1799,7 +1802,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1816,7 +1819,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1833,7 +1836,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1850,7 +1853,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1884,7 +1887,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1964,10 +1967,10 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2035,7 +2038,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2183,10 +2186,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -2254,7 +2257,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -2288,7 +2291,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -2385,7 +2388,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -2402,10 +2405,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -2473,7 +2476,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -2490,7 +2493,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -2519,7 +2522,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>32</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2553,7 +2556,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>23</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>35</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -2621,10 +2624,10 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2675,7 +2678,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -2692,7 +2695,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -2709,7 +2712,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>31</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>32</v>
       </c>
@@ -2755,7 +2758,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>33</v>
       </c>
@@ -2772,7 +2775,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>23</v>
       </c>
@@ -2806,7 +2809,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -2823,7 +2826,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -2840,10 +2843,10 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -2860,7 +2863,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>19</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -2911,7 +2914,7 @@
         <v>0.72699999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -2928,7 +2931,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>31</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>32</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -2991,7 +2994,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>34</v>
       </c>
@@ -3008,7 +3011,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>23</v>
       </c>
@@ -3025,7 +3028,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>35</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -3059,10 +3062,10 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>15</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -3096,7 +3099,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>19</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>20</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>32</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>33</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>34</v>
       </c>
@@ -3215,7 +3218,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>23</v>
       </c>
@@ -3232,7 +3235,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>35</v>
       </c>
@@ -3249,7 +3252,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>36</v>
       </c>
@@ -3266,10 +3269,10 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -3303,7 +3306,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -3320,7 +3323,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -3337,7 +3340,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>28</v>
       </c>
@@ -3354,7 +3357,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>31</v>
       </c>
@@ -3371,7 +3374,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>32</v>
       </c>
@@ -3388,7 +3391,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>33</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -3434,7 +3437,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>23</v>
       </c>
@@ -3451,7 +3454,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>35</v>
       </c>
@@ -3468,7 +3471,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>36</v>
       </c>
@@ -3485,10 +3488,10 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -3505,7 +3508,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>19</v>
       </c>
@@ -3539,7 +3542,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -3556,7 +3559,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>28</v>
       </c>
@@ -3573,7 +3576,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -3590,7 +3593,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>32</v>
       </c>
@@ -3607,7 +3610,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>33</v>
       </c>
@@ -3624,7 +3627,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>34</v>
       </c>
@@ -3641,7 +3644,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>23</v>
       </c>
@@ -3658,7 +3661,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>35</v>
       </c>
@@ -3687,7 +3690,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>36</v>
       </c>
@@ -3715,19 +3718,19 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -3774,7 +3777,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3820,7 +3823,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3866,7 +3869,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3912,7 +3915,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3958,7 +3961,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -4004,7 +4007,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4050,7 +4053,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -4096,7 +4099,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -4142,7 +4145,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -4188,7 +4191,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -4234,7 +4237,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -4264,7 +4267,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -4294,7 +4297,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -4334,7 +4337,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -4358,7 +4361,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -4382,7 +4385,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -4406,13 +4409,18 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>66</v>
       </c>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
draft of LSTM model generator
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todds\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:40009_{CD32B16C-7DED-40CD-BACE-1126F2EAFF7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A2EABAD4-1F11-4F53-A128-8669F7CACB79}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="8805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14712" windowHeight="8808" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -1096,14 +1096,14 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1219,10 +1219,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>782.77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1302,10 +1302,10 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1373,10 +1373,10 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>0.61899999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1529,10 +1529,10 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1748,10 +1748,10 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1967,10 +1967,10 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2186,10 +2186,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -2405,10 +2405,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>32</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>23</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>35</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -2624,10 +2624,10 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>31</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>32</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>33</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>23</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -2843,10 +2843,10 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>19</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>0.72699999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>31</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>32</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>34</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>23</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>35</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -3062,10 +3062,10 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>15</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>19</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>20</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>32</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>33</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>34</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>23</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>35</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>36</v>
       </c>
@@ -3269,10 +3269,10 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>28</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>31</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>32</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>33</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>23</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>35</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>36</v>
       </c>
@@ -3488,10 +3488,10 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>19</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>28</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>32</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>33</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>34</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>23</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>35</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>36</v>
       </c>
@@ -3718,19 +3718,19 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="9.796875" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3823,7 +3823,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3869,7 +3869,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3915,7 +3915,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -4007,7 +4007,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4053,7 +4053,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -4099,7 +4099,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -4191,7 +4191,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -4237,7 +4237,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -4297,7 +4297,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -4337,7 +4337,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -4361,7 +4361,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -4385,7 +4385,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -4409,18 +4409,18 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>66</v>
       </c>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
begun adding to this
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulbirmiwal/Documents/UWMSDS/Capstone/ProjectDir2/EnvNoiseDetector/data/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:40009_{CD32B16C-7DED-40CD-BACE-1126F2EAFF7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A2EABAD4-1F11-4F53-A128-8669F7CACB79}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14712" windowHeight="8808" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9220" yWindow="460" windowWidth="15980" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
     <sheet name="Plot" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="74">
   <si>
     <t>ModelType</t>
   </si>
@@ -236,12 +236,27 @@
   </si>
   <si>
     <t>* All comtaminated signals have signal-to-noise of 6 dB</t>
+  </si>
+  <si>
+    <t>Wvl. (CF2, L3) Entropy-Var-Subband T1 [13 Feat]</t>
+  </si>
+  <si>
+    <t>Subspace KNN</t>
+  </si>
+  <si>
+    <t>FinalWaveletFeatures_PCA_SS_coif2_L3.mat</t>
+  </si>
+  <si>
+    <t>FinalWaveletFeatures_PCA_SS_CF2_L5.mat</t>
+  </si>
+  <si>
+    <t>Wvl. (CF2, L4) Entropy-Var-Subband T1 [17 Feat]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -722,12 +737,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1089,21 +1105,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I187"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E182" sqref="E182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1178,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1190,7 +1207,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1219,10 +1236,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1239,7 +1256,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1268,7 +1285,7 @@
         <v>782.77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1285,7 +1302,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1302,10 +1319,10 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1322,7 +1339,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1339,7 +1356,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1356,7 +1373,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1373,10 +1390,10 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1393,7 +1410,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1410,7 +1427,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1427,7 +1444,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1444,7 +1461,7 @@
         <v>0.61899999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1461,7 +1478,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1478,7 +1495,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1495,7 +1512,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1512,7 +1529,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1529,10 +1546,10 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1549,7 +1566,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1583,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1583,7 +1600,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1600,7 +1617,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1617,7 +1634,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1634,7 +1651,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1651,7 +1668,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1668,7 +1685,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1714,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1714,7 +1731,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1731,7 +1748,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1748,10 +1765,10 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1768,7 +1785,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1785,7 +1802,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1802,7 +1819,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1819,7 +1836,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1836,7 +1853,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1853,7 +1870,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -1870,7 +1887,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1887,7 +1904,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1916,7 +1933,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1933,7 +1950,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1950,7 +1967,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1967,10 +1984,10 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -1987,7 +2004,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2004,7 +2021,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -2021,7 +2038,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2038,7 +2055,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -2055,7 +2072,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -2072,7 +2089,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -2089,7 +2106,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -2106,7 +2123,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2135,7 +2152,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -2152,7 +2169,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -2169,7 +2186,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2186,10 +2203,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -2206,7 +2223,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -2223,7 +2240,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2240,7 +2257,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -2257,7 +2274,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -2274,7 +2291,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -2291,7 +2308,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -2308,7 +2325,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -2325,7 +2342,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -2354,7 +2371,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -2371,7 +2388,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -2388,7 +2405,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -2405,10 +2422,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -2425,7 +2442,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -2442,7 +2459,7 @@
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2459,7 +2476,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -2476,7 +2493,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -2493,7 +2510,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -2522,7 +2539,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>32</v>
       </c>
@@ -2539,7 +2556,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2556,7 +2573,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -2573,7 +2590,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>23</v>
       </c>
@@ -2590,7 +2607,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>35</v>
       </c>
@@ -2607,7 +2624,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -2624,10 +2641,10 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -2644,7 +2661,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -2661,7 +2678,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2678,7 +2695,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -2695,7 +2712,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -2712,7 +2729,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>31</v>
       </c>
@@ -2741,7 +2758,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>32</v>
       </c>
@@ -2758,7 +2775,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>33</v>
       </c>
@@ -2775,7 +2792,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -2792,7 +2809,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>23</v>
       </c>
@@ -2809,7 +2826,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -2826,7 +2843,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -2843,10 +2860,10 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -2863,7 +2880,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -2880,7 +2897,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>19</v>
       </c>
@@ -2897,7 +2914,7 @@
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -2914,7 +2931,7 @@
         <v>0.72699999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -2931,7 +2948,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>31</v>
       </c>
@@ -2960,7 +2977,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>32</v>
       </c>
@@ -2977,7 +2994,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -2994,7 +3011,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>34</v>
       </c>
@@ -3011,7 +3028,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>23</v>
       </c>
@@ -3028,7 +3045,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>35</v>
       </c>
@@ -3045,7 +3062,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -3062,10 +3079,10 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>15</v>
       </c>
@@ -3082,7 +3099,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -3099,7 +3116,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>19</v>
       </c>
@@ -3116,7 +3133,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>20</v>
       </c>
@@ -3133,7 +3150,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -3150,7 +3167,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -3167,7 +3184,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>32</v>
       </c>
@@ -3184,7 +3201,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>33</v>
       </c>
@@ -3201,7 +3218,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>34</v>
       </c>
@@ -3218,7 +3235,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>23</v>
       </c>
@@ -3235,7 +3252,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>35</v>
       </c>
@@ -3252,7 +3269,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>36</v>
       </c>
@@ -3269,10 +3286,10 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -3289,7 +3306,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -3306,7 +3323,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -3323,7 +3340,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -3340,7 +3357,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>28</v>
       </c>
@@ -3357,7 +3374,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>31</v>
       </c>
@@ -3374,7 +3391,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>32</v>
       </c>
@@ -3391,7 +3408,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>33</v>
       </c>
@@ -3408,7 +3425,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -3437,7 +3454,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>23</v>
       </c>
@@ -3454,7 +3471,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>35</v>
       </c>
@@ -3471,7 +3488,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>36</v>
       </c>
@@ -3488,10 +3505,10 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -3508,7 +3525,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -3525,7 +3542,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>19</v>
       </c>
@@ -3542,7 +3559,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -3559,7 +3576,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>28</v>
       </c>
@@ -3576,7 +3593,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -3593,7 +3610,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>32</v>
       </c>
@@ -3610,7 +3627,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>33</v>
       </c>
@@ -3627,7 +3644,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>34</v>
       </c>
@@ -3644,7 +3661,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>23</v>
       </c>
@@ -3661,7 +3678,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>35</v>
       </c>
@@ -3690,7 +3707,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>36</v>
       </c>
@@ -3705,6 +3722,448 @@
       </c>
       <c r="E154" s="1">
         <v>0.76400000000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>15</v>
+      </c>
+      <c r="B159" t="s">
+        <v>16</v>
+      </c>
+      <c r="C159" t="s">
+        <v>69</v>
+      </c>
+      <c r="D159" t="s">
+        <v>71</v>
+      </c>
+      <c r="E159" s="3">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>18</v>
+      </c>
+      <c r="B160" t="s">
+        <v>16</v>
+      </c>
+      <c r="C160" t="s">
+        <v>69</v>
+      </c>
+      <c r="D160" t="s">
+        <v>71</v>
+      </c>
+      <c r="E160" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>19</v>
+      </c>
+      <c r="B161" t="s">
+        <v>16</v>
+      </c>
+      <c r="C161" t="s">
+        <v>69</v>
+      </c>
+      <c r="D161" t="s">
+        <v>71</v>
+      </c>
+      <c r="E161" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>20</v>
+      </c>
+      <c r="B162" t="s">
+        <v>16</v>
+      </c>
+      <c r="C162" t="s">
+        <v>69</v>
+      </c>
+      <c r="D162" t="s">
+        <v>71</v>
+      </c>
+      <c r="E162" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>28</v>
+      </c>
+      <c r="B163" t="s">
+        <v>16</v>
+      </c>
+      <c r="C163" t="s">
+        <v>69</v>
+      </c>
+      <c r="D163" t="s">
+        <v>71</v>
+      </c>
+      <c r="E163" s="3">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>31</v>
+      </c>
+      <c r="B164" t="s">
+        <v>16</v>
+      </c>
+      <c r="C164" t="s">
+        <v>69</v>
+      </c>
+      <c r="D164" t="s">
+        <v>71</v>
+      </c>
+      <c r="E164" s="3">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>32</v>
+      </c>
+      <c r="B165" t="s">
+        <v>16</v>
+      </c>
+      <c r="C165" t="s">
+        <v>69</v>
+      </c>
+      <c r="D165" t="s">
+        <v>71</v>
+      </c>
+      <c r="E165" s="3">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>33</v>
+      </c>
+      <c r="B166" t="s">
+        <v>16</v>
+      </c>
+      <c r="C166" t="s">
+        <v>69</v>
+      </c>
+      <c r="D166" t="s">
+        <v>71</v>
+      </c>
+      <c r="E166" s="3">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>34</v>
+      </c>
+      <c r="B167" t="s">
+        <v>16</v>
+      </c>
+      <c r="C167" t="s">
+        <v>69</v>
+      </c>
+      <c r="D167" t="s">
+        <v>71</v>
+      </c>
+      <c r="E167" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>23</v>
+      </c>
+      <c r="B168" t="s">
+        <v>16</v>
+      </c>
+      <c r="C168" t="s">
+        <v>69</v>
+      </c>
+      <c r="D168" t="s">
+        <v>71</v>
+      </c>
+      <c r="E168" s="3">
+        <v>0.83899999999999997</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>35</v>
+      </c>
+      <c r="B169" t="s">
+        <v>16</v>
+      </c>
+      <c r="C169" t="s">
+        <v>69</v>
+      </c>
+      <c r="D169" t="s">
+        <v>71</v>
+      </c>
+      <c r="E169" s="3">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>36</v>
+      </c>
+      <c r="B170" t="s">
+        <v>16</v>
+      </c>
+      <c r="C170" t="s">
+        <v>69</v>
+      </c>
+      <c r="D170" t="s">
+        <v>71</v>
+      </c>
+      <c r="E170" s="3">
+        <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>70</v>
+      </c>
+      <c r="B171" t="s">
+        <v>16</v>
+      </c>
+      <c r="C171" t="s">
+        <v>69</v>
+      </c>
+      <c r="D171" t="s">
+        <v>71</v>
+      </c>
+      <c r="E171" s="3">
+        <v>0.81399999999999995</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>15</v>
+      </c>
+      <c r="B175" t="s">
+        <v>16</v>
+      </c>
+      <c r="C175" t="s">
+        <v>73</v>
+      </c>
+      <c r="D175" t="s">
+        <v>72</v>
+      </c>
+      <c r="E175" s="1">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>18</v>
+      </c>
+      <c r="B176" t="s">
+        <v>16</v>
+      </c>
+      <c r="C176" t="s">
+        <v>73</v>
+      </c>
+      <c r="D176" t="s">
+        <v>72</v>
+      </c>
+      <c r="E176" s="1">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>19</v>
+      </c>
+      <c r="B177" t="s">
+        <v>16</v>
+      </c>
+      <c r="C177" t="s">
+        <v>73</v>
+      </c>
+      <c r="D177" t="s">
+        <v>72</v>
+      </c>
+      <c r="E177" s="1">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>20</v>
+      </c>
+      <c r="B178" t="s">
+        <v>16</v>
+      </c>
+      <c r="C178" t="s">
+        <v>73</v>
+      </c>
+      <c r="D178" t="s">
+        <v>72</v>
+      </c>
+      <c r="E178" s="1">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>28</v>
+      </c>
+      <c r="B179" t="s">
+        <v>16</v>
+      </c>
+      <c r="C179" t="s">
+        <v>73</v>
+      </c>
+      <c r="D179" t="s">
+        <v>72</v>
+      </c>
+      <c r="E179" s="1">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>31</v>
+      </c>
+      <c r="B180" t="s">
+        <v>16</v>
+      </c>
+      <c r="C180" t="s">
+        <v>73</v>
+      </c>
+      <c r="D180" t="s">
+        <v>72</v>
+      </c>
+      <c r="E180" s="1">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>32</v>
+      </c>
+      <c r="B181" t="s">
+        <v>16</v>
+      </c>
+      <c r="C181" t="s">
+        <v>73</v>
+      </c>
+      <c r="D181" t="s">
+        <v>72</v>
+      </c>
+      <c r="E181" s="1">
+        <v>0.94899999999999995</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>33</v>
+      </c>
+      <c r="B182" t="s">
+        <v>16</v>
+      </c>
+      <c r="C182" t="s">
+        <v>73</v>
+      </c>
+      <c r="D182" t="s">
+        <v>72</v>
+      </c>
+      <c r="E182" s="1">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>34</v>
+      </c>
+      <c r="B183" t="s">
+        <v>16</v>
+      </c>
+      <c r="C183" t="s">
+        <v>73</v>
+      </c>
+      <c r="D183" t="s">
+        <v>72</v>
+      </c>
+      <c r="E183" s="1">
+        <v>0.96599999999999997</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>23</v>
+      </c>
+      <c r="B184" t="s">
+        <v>16</v>
+      </c>
+      <c r="C184" t="s">
+        <v>73</v>
+      </c>
+      <c r="D184" t="s">
+        <v>72</v>
+      </c>
+      <c r="E184" s="1">
+        <v>0.84699999999999998</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>35</v>
+      </c>
+      <c r="B185" t="s">
+        <v>16</v>
+      </c>
+      <c r="C185" t="s">
+        <v>73</v>
+      </c>
+      <c r="D185" t="s">
+        <v>72</v>
+      </c>
+      <c r="E185" s="1">
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>36</v>
+      </c>
+      <c r="B186" t="s">
+        <v>16</v>
+      </c>
+      <c r="C186" t="s">
+        <v>73</v>
+      </c>
+      <c r="D186" t="s">
+        <v>72</v>
+      </c>
+      <c r="E186" s="1">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>70</v>
+      </c>
+      <c r="B187" t="s">
+        <v>16</v>
+      </c>
+      <c r="C187" t="s">
+        <v>73</v>
+      </c>
+      <c r="D187" t="s">
+        <v>72</v>
+      </c>
+      <c r="E187" s="1">
+        <v>0.92400000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -3714,23 +4173,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -3777,7 +4236,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3823,7 +4282,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3869,7 +4328,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3915,7 +4374,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3961,7 +4420,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -4007,7 +4466,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4053,7 +4512,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -4099,7 +4558,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -4145,7 +4604,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -4191,7 +4650,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -4237,7 +4696,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -4267,7 +4726,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -4297,7 +4756,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -4337,7 +4796,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -4361,7 +4820,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -4385,7 +4844,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -4409,18 +4868,18 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>66</v>
       </c>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Add Wavelet Scalogram bag of features and model results
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -1,34 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulbirmiwal/Documents/UWMSDS/Capstone/ProjectDir2/EnvNoiseDetector/data/Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UW\Project\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137B159A-435A-4D47-861B-9B215CB41435}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9220" yWindow="460" windowWidth="15980" windowHeight="13380"/>
+    <workbookView xWindow="9225" yWindow="465" windowWidth="15975" windowHeight="13380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
     <sheet name="Plot" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="82">
   <si>
     <t>ModelType</t>
   </si>
@@ -256,12 +249,30 @@
   </si>
   <si>
     <t xml:space="preserve">Subspace Descriminant </t>
+  </si>
+  <si>
+    <t>SNR 6 Wavelet Scalogram Bag of Features - 1s</t>
+  </si>
+  <si>
+    <t>FeaturesSNR6WaveletScalogramSURFOneSecv1.mat</t>
+  </si>
+  <si>
+    <t>SNR 6 Wavelet Scalogram Bag of Features - 3s</t>
+  </si>
+  <si>
+    <t>FeaturesSNR6WaveletScalogramSURFThreeSecv1.mat</t>
+  </si>
+  <si>
+    <t>SNR 6 Wavelet Scalogram Bag of Features - 5s</t>
+  </si>
+  <si>
+    <t>FeaturesSNR6WaveletScalogramSURFFiveSecv1.mat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -794,7 +805,19 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1110,22 +1133,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I201"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E202" sqref="E202"/>
+    <sheetView topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E159" sqref="E159:E171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1206,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1212,7 +1235,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1241,10 +1264,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1261,7 +1284,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1290,7 +1313,7 @@
         <v>782.77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1307,7 +1330,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1324,10 +1347,10 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1344,7 +1367,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1361,7 +1384,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1378,7 +1401,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1395,10 +1418,10 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1415,7 +1438,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1432,7 +1455,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1449,7 +1472,7 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1466,7 +1489,7 @@
         <v>0.61899999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1483,7 +1506,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1500,7 +1523,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1517,7 +1540,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1534,7 +1557,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1551,10 +1574,10 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1571,7 +1594,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1588,7 +1611,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1605,7 +1628,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1622,7 +1645,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1639,7 +1662,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1656,7 +1679,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1673,7 +1696,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1690,7 +1713,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1719,7 +1742,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1736,7 +1759,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1753,7 +1776,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1770,10 +1793,10 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1790,7 +1813,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1807,7 +1830,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1824,7 +1847,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1841,7 +1864,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1858,7 +1881,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1875,7 +1898,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -1892,7 +1915,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1909,7 +1932,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1938,7 +1961,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1955,7 +1978,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1972,7 +1995,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1989,10 +2012,10 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2009,7 +2032,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2026,7 +2049,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -2043,7 +2066,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2060,7 +2083,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -2077,7 +2100,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -2094,7 +2117,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -2111,7 +2134,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -2128,7 +2151,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2157,7 +2180,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -2174,7 +2197,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -2191,7 +2214,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2208,10 +2231,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -2228,7 +2251,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -2245,7 +2268,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2262,7 +2285,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -2279,7 +2302,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -2296,7 +2319,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -2313,7 +2336,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -2330,7 +2353,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -2347,7 +2370,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -2376,7 +2399,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -2393,7 +2416,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -2410,7 +2433,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -2427,10 +2450,10 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -2447,7 +2470,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -2464,7 +2487,7 @@
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2481,7 +2504,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -2498,7 +2521,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -2515,7 +2538,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -2544,7 +2567,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>32</v>
       </c>
@@ -2561,7 +2584,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2578,7 +2601,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -2595,7 +2618,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>23</v>
       </c>
@@ -2612,7 +2635,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>35</v>
       </c>
@@ -2629,7 +2652,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -2646,10 +2669,10 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -2666,7 +2689,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -2683,7 +2706,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2700,7 +2723,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -2717,7 +2740,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -2734,7 +2757,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>31</v>
       </c>
@@ -2763,7 +2786,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>32</v>
       </c>
@@ -2780,7 +2803,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>33</v>
       </c>
@@ -2797,7 +2820,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -2814,7 +2837,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>23</v>
       </c>
@@ -2831,7 +2854,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -2848,7 +2871,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -2865,10 +2888,10 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -2885,7 +2908,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -2902,7 +2925,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>19</v>
       </c>
@@ -2919,7 +2942,7 @@
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -2936,7 +2959,7 @@
         <v>0.72699999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -2953,7 +2976,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>31</v>
       </c>
@@ -2982,7 +3005,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>32</v>
       </c>
@@ -2999,7 +3022,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -3016,7 +3039,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>34</v>
       </c>
@@ -3033,7 +3056,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>23</v>
       </c>
@@ -3050,7 +3073,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>35</v>
       </c>
@@ -3067,7 +3090,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -3084,10 +3107,10 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>15</v>
       </c>
@@ -3104,7 +3127,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -3121,7 +3144,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>19</v>
       </c>
@@ -3138,7 +3161,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>20</v>
       </c>
@@ -3155,7 +3178,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -3172,7 +3195,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -3189,7 +3212,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>32</v>
       </c>
@@ -3206,7 +3229,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>33</v>
       </c>
@@ -3223,7 +3246,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>34</v>
       </c>
@@ -3240,7 +3263,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>23</v>
       </c>
@@ -3257,7 +3280,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>35</v>
       </c>
@@ -3274,7 +3297,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>36</v>
       </c>
@@ -3291,10 +3314,10 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -3311,7 +3334,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -3328,7 +3351,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -3345,7 +3368,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -3362,7 +3385,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>28</v>
       </c>
@@ -3379,7 +3402,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>31</v>
       </c>
@@ -3396,7 +3419,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>32</v>
       </c>
@@ -3413,7 +3436,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>33</v>
       </c>
@@ -3430,7 +3453,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -3459,7 +3482,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>23</v>
       </c>
@@ -3476,7 +3499,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>35</v>
       </c>
@@ -3493,7 +3516,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>36</v>
       </c>
@@ -3510,10 +3533,10 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -3530,7 +3553,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -3547,7 +3570,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>19</v>
       </c>
@@ -3564,7 +3587,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -3581,7 +3604,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>28</v>
       </c>
@@ -3598,7 +3621,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -3615,7 +3638,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>32</v>
       </c>
@@ -3632,7 +3655,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>33</v>
       </c>
@@ -3649,7 +3672,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>34</v>
       </c>
@@ -3666,7 +3689,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>23</v>
       </c>
@@ -3683,7 +3706,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>35</v>
       </c>
@@ -3712,7 +3735,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>36</v>
       </c>
@@ -3729,7 +3752,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>15</v>
       </c>
@@ -3746,7 +3769,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>18</v>
       </c>
@@ -3763,7 +3786,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>19</v>
       </c>
@@ -3780,7 +3803,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>20</v>
       </c>
@@ -3797,7 +3820,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>28</v>
       </c>
@@ -3814,7 +3837,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>31</v>
       </c>
@@ -3831,7 +3854,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>32</v>
       </c>
@@ -3848,7 +3871,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>33</v>
       </c>
@@ -3865,7 +3888,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>34</v>
       </c>
@@ -3882,7 +3905,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>23</v>
       </c>
@@ -3899,7 +3922,7 @@
         <v>0.83899999999999997</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>35</v>
       </c>
@@ -3916,7 +3939,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -3933,7 +3956,7 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>70</v>
       </c>
@@ -3950,7 +3973,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>15</v>
       </c>
@@ -3967,7 +3990,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>18</v>
       </c>
@@ -3984,7 +4007,7 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>19</v>
       </c>
@@ -4001,7 +4024,7 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>20</v>
       </c>
@@ -4018,7 +4041,7 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>28</v>
       </c>
@@ -4035,7 +4058,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>31</v>
       </c>
@@ -4052,7 +4075,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>32</v>
       </c>
@@ -4069,7 +4092,7 @@
         <v>0.94899999999999995</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>33</v>
       </c>
@@ -4086,7 +4109,7 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>34</v>
       </c>
@@ -4103,7 +4126,7 @@
         <v>0.96599999999999997</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>23</v>
       </c>
@@ -4120,7 +4143,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>35</v>
       </c>
@@ -4137,7 +4160,7 @@
         <v>0.95799999999999996</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>36</v>
       </c>
@@ -4154,7 +4177,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>70</v>
       </c>
@@ -4171,7 +4194,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>15</v>
       </c>
@@ -4185,7 +4208,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>18</v>
       </c>
@@ -4199,7 +4222,7 @@
         <v>0.83899999999999997</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>19</v>
       </c>
@@ -4213,7 +4236,7 @@
         <v>0.83899999999999997</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>20</v>
       </c>
@@ -4227,7 +4250,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>28</v>
       </c>
@@ -4241,7 +4264,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>31</v>
       </c>
@@ -4255,7 +4278,7 @@
         <v>0.85599999999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>32</v>
       </c>
@@ -4269,7 +4292,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>33</v>
       </c>
@@ -4283,7 +4306,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>34</v>
       </c>
@@ -4297,7 +4320,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>23</v>
       </c>
@@ -4311,7 +4334,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>35</v>
       </c>
@@ -4325,7 +4348,7 @@
         <v>0.72899999999999998</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>36</v>
       </c>
@@ -4339,7 +4362,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>75</v>
       </c>
@@ -4351,6 +4374,654 @@
       </c>
       <c r="E201" s="1">
         <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>15</v>
+      </c>
+      <c r="B203" t="s">
+        <v>16</v>
+      </c>
+      <c r="C203" t="s">
+        <v>76</v>
+      </c>
+      <c r="D203" t="s">
+        <v>77</v>
+      </c>
+      <c r="E203" s="3">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>18</v>
+      </c>
+      <c r="B204" t="s">
+        <v>16</v>
+      </c>
+      <c r="C204" t="s">
+        <v>76</v>
+      </c>
+      <c r="D204" t="s">
+        <v>77</v>
+      </c>
+      <c r="E204" s="3">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>19</v>
+      </c>
+      <c r="B205" t="s">
+        <v>16</v>
+      </c>
+      <c r="C205" t="s">
+        <v>76</v>
+      </c>
+      <c r="D205" t="s">
+        <v>77</v>
+      </c>
+      <c r="E205" s="3">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>20</v>
+      </c>
+      <c r="B206" t="s">
+        <v>16</v>
+      </c>
+      <c r="C206" t="s">
+        <v>76</v>
+      </c>
+      <c r="D206" t="s">
+        <v>77</v>
+      </c>
+      <c r="E206" s="3">
+        <v>0.73299999999999998</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>28</v>
+      </c>
+      <c r="B207" t="s">
+        <v>16</v>
+      </c>
+      <c r="C207" t="s">
+        <v>76</v>
+      </c>
+      <c r="D207" t="s">
+        <v>77</v>
+      </c>
+      <c r="E207" s="3">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>31</v>
+      </c>
+      <c r="B208" t="s">
+        <v>16</v>
+      </c>
+      <c r="C208" t="s">
+        <v>76</v>
+      </c>
+      <c r="D208" t="s">
+        <v>77</v>
+      </c>
+      <c r="E208" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>32</v>
+      </c>
+      <c r="B209" t="s">
+        <v>16</v>
+      </c>
+      <c r="C209" t="s">
+        <v>76</v>
+      </c>
+      <c r="D209" t="s">
+        <v>77</v>
+      </c>
+      <c r="E209" s="3">
+        <v>0.83099999999999996</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>33</v>
+      </c>
+      <c r="B210" t="s">
+        <v>16</v>
+      </c>
+      <c r="C210" t="s">
+        <v>76</v>
+      </c>
+      <c r="D210" t="s">
+        <v>77</v>
+      </c>
+      <c r="E210" s="3">
+        <v>0.86399999999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>34</v>
+      </c>
+      <c r="B211" t="s">
+        <v>16</v>
+      </c>
+      <c r="C211" t="s">
+        <v>76</v>
+      </c>
+      <c r="D211" t="s">
+        <v>77</v>
+      </c>
+      <c r="E211" s="3">
+        <v>0.871</v>
+      </c>
+      <c r="F211">
+        <v>1801</v>
+      </c>
+      <c r="G211">
+        <v>217</v>
+      </c>
+      <c r="H211">
+        <v>303</v>
+      </c>
+      <c r="I211">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>23</v>
+      </c>
+      <c r="B212" t="s">
+        <v>16</v>
+      </c>
+      <c r="C212" t="s">
+        <v>76</v>
+      </c>
+      <c r="D212" t="s">
+        <v>77</v>
+      </c>
+      <c r="E212" s="3">
+        <v>0.60499999999999998</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>35</v>
+      </c>
+      <c r="B213" t="s">
+        <v>16</v>
+      </c>
+      <c r="C213" t="s">
+        <v>76</v>
+      </c>
+      <c r="D213" t="s">
+        <v>77</v>
+      </c>
+      <c r="E213" s="3">
+        <v>0.86099999999999999</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>36</v>
+      </c>
+      <c r="B214" t="s">
+        <v>16</v>
+      </c>
+      <c r="C214" t="s">
+        <v>76</v>
+      </c>
+      <c r="D214" t="s">
+        <v>77</v>
+      </c>
+      <c r="E214" s="3">
+        <v>0.79900000000000004</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>15</v>
+      </c>
+      <c r="B216" t="s">
+        <v>16</v>
+      </c>
+      <c r="C216" t="s">
+        <v>78</v>
+      </c>
+      <c r="D216" t="s">
+        <v>79</v>
+      </c>
+      <c r="E216" s="3">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>18</v>
+      </c>
+      <c r="B217" t="s">
+        <v>16</v>
+      </c>
+      <c r="C217" t="s">
+        <v>78</v>
+      </c>
+      <c r="D217" t="s">
+        <v>79</v>
+      </c>
+      <c r="E217" s="3">
+        <v>0.73199999999999998</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>19</v>
+      </c>
+      <c r="B218" t="s">
+        <v>16</v>
+      </c>
+      <c r="C218" t="s">
+        <v>78</v>
+      </c>
+      <c r="D218" t="s">
+        <v>79</v>
+      </c>
+      <c r="E218" s="3">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>20</v>
+      </c>
+      <c r="B219" t="s">
+        <v>16</v>
+      </c>
+      <c r="C219" t="s">
+        <v>78</v>
+      </c>
+      <c r="D219" t="s">
+        <v>79</v>
+      </c>
+      <c r="E219" s="3">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>28</v>
+      </c>
+      <c r="B220" t="s">
+        <v>16</v>
+      </c>
+      <c r="C220" t="s">
+        <v>78</v>
+      </c>
+      <c r="D220" t="s">
+        <v>79</v>
+      </c>
+      <c r="E220" s="3">
+        <v>0.84799999999999998</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>31</v>
+      </c>
+      <c r="B221" t="s">
+        <v>16</v>
+      </c>
+      <c r="C221" t="s">
+        <v>78</v>
+      </c>
+      <c r="D221" t="s">
+        <v>79</v>
+      </c>
+      <c r="E221" s="3">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>32</v>
+      </c>
+      <c r="B222" t="s">
+        <v>16</v>
+      </c>
+      <c r="C222" t="s">
+        <v>78</v>
+      </c>
+      <c r="D222" t="s">
+        <v>79</v>
+      </c>
+      <c r="E222" s="3">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>33</v>
+      </c>
+      <c r="B223" t="s">
+        <v>16</v>
+      </c>
+      <c r="C223" t="s">
+        <v>78</v>
+      </c>
+      <c r="D223" t="s">
+        <v>79</v>
+      </c>
+      <c r="E223" s="3">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>34</v>
+      </c>
+      <c r="B224" t="s">
+        <v>16</v>
+      </c>
+      <c r="C224" t="s">
+        <v>78</v>
+      </c>
+      <c r="D224" t="s">
+        <v>79</v>
+      </c>
+      <c r="E224" s="3">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="F224">
+        <v>589</v>
+      </c>
+      <c r="G224">
+        <v>62</v>
+      </c>
+      <c r="H224">
+        <v>87</v>
+      </c>
+      <c r="I224">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>23</v>
+      </c>
+      <c r="B225" t="s">
+        <v>16</v>
+      </c>
+      <c r="C225" t="s">
+        <v>78</v>
+      </c>
+      <c r="D225" t="s">
+        <v>79</v>
+      </c>
+      <c r="E225" s="3">
+        <v>0.59099999999999997</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>35</v>
+      </c>
+      <c r="B226" t="s">
+        <v>16</v>
+      </c>
+      <c r="C226" t="s">
+        <v>78</v>
+      </c>
+      <c r="D226" t="s">
+        <v>79</v>
+      </c>
+      <c r="E226" s="3">
+        <v>0.879</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>36</v>
+      </c>
+      <c r="B227" t="s">
+        <v>16</v>
+      </c>
+      <c r="C227" t="s">
+        <v>78</v>
+      </c>
+      <c r="D227" t="s">
+        <v>79</v>
+      </c>
+      <c r="E227" s="3">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>15</v>
+      </c>
+      <c r="B229" t="s">
+        <v>16</v>
+      </c>
+      <c r="C229" t="s">
+        <v>80</v>
+      </c>
+      <c r="D229" t="s">
+        <v>81</v>
+      </c>
+      <c r="E229" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>18</v>
+      </c>
+      <c r="B230" t="s">
+        <v>16</v>
+      </c>
+      <c r="C230" t="s">
+        <v>80</v>
+      </c>
+      <c r="D230" t="s">
+        <v>81</v>
+      </c>
+      <c r="E230" s="3">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>19</v>
+      </c>
+      <c r="B231" t="s">
+        <v>16</v>
+      </c>
+      <c r="C231" t="s">
+        <v>80</v>
+      </c>
+      <c r="D231" t="s">
+        <v>81</v>
+      </c>
+      <c r="E231" s="3">
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>20</v>
+      </c>
+      <c r="B232" t="s">
+        <v>16</v>
+      </c>
+      <c r="C232" t="s">
+        <v>80</v>
+      </c>
+      <c r="D232" t="s">
+        <v>81</v>
+      </c>
+      <c r="E232" s="3">
+        <v>0.70599999999999996</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>28</v>
+      </c>
+      <c r="B233" t="s">
+        <v>16</v>
+      </c>
+      <c r="C233" t="s">
+        <v>80</v>
+      </c>
+      <c r="D233" t="s">
+        <v>81</v>
+      </c>
+      <c r="E233" s="3">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>31</v>
+      </c>
+      <c r="B234" t="s">
+        <v>16</v>
+      </c>
+      <c r="C234" t="s">
+        <v>80</v>
+      </c>
+      <c r="D234" t="s">
+        <v>81</v>
+      </c>
+      <c r="E234" s="3">
+        <v>0.81699999999999995</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>32</v>
+      </c>
+      <c r="B235" t="s">
+        <v>16</v>
+      </c>
+      <c r="C235" t="s">
+        <v>80</v>
+      </c>
+      <c r="D235" t="s">
+        <v>81</v>
+      </c>
+      <c r="E235" s="3">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>33</v>
+      </c>
+      <c r="B236" t="s">
+        <v>16</v>
+      </c>
+      <c r="C236" t="s">
+        <v>80</v>
+      </c>
+      <c r="D236" t="s">
+        <v>81</v>
+      </c>
+      <c r="E236" s="3">
+        <v>0.89400000000000002</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>34</v>
+      </c>
+      <c r="B237" t="s">
+        <v>16</v>
+      </c>
+      <c r="C237" t="s">
+        <v>80</v>
+      </c>
+      <c r="D237" t="s">
+        <v>81</v>
+      </c>
+      <c r="E237" s="3">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="F237">
+        <v>294</v>
+      </c>
+      <c r="G237">
+        <v>26</v>
+      </c>
+      <c r="H237">
+        <v>32</v>
+      </c>
+      <c r="I237">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>23</v>
+      </c>
+      <c r="B238" t="s">
+        <v>16</v>
+      </c>
+      <c r="C238" t="s">
+        <v>80</v>
+      </c>
+      <c r="D238" t="s">
+        <v>81</v>
+      </c>
+      <c r="E238" s="3">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>35</v>
+      </c>
+      <c r="B239" t="s">
+        <v>16</v>
+      </c>
+      <c r="C239" t="s">
+        <v>80</v>
+      </c>
+      <c r="D239" t="s">
+        <v>81</v>
+      </c>
+      <c r="E239" s="3">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>36</v>
+      </c>
+      <c r="B240" t="s">
+        <v>16</v>
+      </c>
+      <c r="C240" t="s">
+        <v>80</v>
+      </c>
+      <c r="D240" t="s">
+        <v>81</v>
+      </c>
+      <c r="E240" s="3">
+        <v>0.81599999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -4360,23 +5031,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="9.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -4422,8 +5093,11 @@
       <c r="P1" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -4469,7 +5143,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4515,7 +5189,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -4561,7 +5235,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -4607,7 +5281,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -4653,7 +5327,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4699,7 +5373,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -4745,7 +5419,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -4791,7 +5465,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -4837,7 +5511,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -4883,7 +5557,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -4913,7 +5587,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -4943,7 +5617,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -4983,22 +5657,46 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="B15" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.755</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.871</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0.79900000000000004</v>
+      </c>
       <c r="N15" s="1">
         <v>0.92900000000000005</v>
       </c>
@@ -5007,22 +5705,46 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="B16" s="3">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.753</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.877</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.879</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.81599999999999995</v>
+      </c>
       <c r="N16" s="1">
         <v>0.85099999999999998</v>
       </c>
@@ -5031,22 +5753,46 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="B17" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.877</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0.81599999999999995</v>
+      </c>
       <c r="N17" s="1">
         <v>0.83299999999999996</v>
       </c>
@@ -5055,26 +5801,180 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.754</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.81399999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>66</v>
       </c>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P17">
-    <cfRule type="top10" dxfId="0" priority="3" rank="3"/>
+  <conditionalFormatting sqref="B2:P14 N15:P15 B16:P17">
+    <cfRule type="top10" dxfId="2" priority="7" rank="3"/>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:M15">
+    <cfRule type="top10" dxfId="1" priority="3" rank="3"/>
     <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:M20 Q18:Q20">
+    <cfRule type="top10" dxfId="0" priority="9" rank="3"/>
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
restored lstm model for cepstral features
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="114_{CCE046F7-4B59-4875-AA44-F1D86BAF471B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{1681C8F5-270A-4E10-B34D-EA6C48AE115A}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="114_{CCE046F7-4B59-4875-AA44-F1D86BAF471B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{8B7880BB-40AB-42A6-BAF3-002927FB6E77}"/>
   <bookViews>
-    <workbookView xWindow="9228" yWindow="468" windowWidth="15972" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9228" yWindow="468" windowWidth="15972" windowHeight="13380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -1170,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C260" sqref="C260"/>
+    <sheetView topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2498,7 +2498,7 @@
         <v>42</v>
       </c>
       <c r="E77" s="1">
-        <v>0.60199999999999998</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="J77" t="s">
         <v>89</v>
@@ -5488,11 +5488,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V10" sqref="V10"/>
+      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5749,7 +5749,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4">
-        <v>0.60199999999999998</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>

</xml_diff>

<commit_message>
Update model resulst with coiflet2 T2 and added entropy
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todds\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulbirmiwal/Documents/UWMSDS/Capstone/ProjectDir/EnvNoiseDetector/data/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="114_{CCE046F7-4B59-4875-AA44-F1D86BAF471B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FEF709F7-E9C7-45AA-8236-44175288FEC7}"/>
   <bookViews>
-    <workbookView xWindow="9225" yWindow="465" windowWidth="15975" windowHeight="13380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="22000" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="88">
   <si>
     <t>ModelType</t>
   </si>
@@ -273,42 +272,6 @@
   </si>
   <si>
     <t>FeaturesWavelets_coif2_Lvl4_T2.mat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Didn't have time to do the latter one with all features, MATLAB crashed and takes 2 hours </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Takeaway: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">This method for feature extraction works better as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>tblock</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve"> increases</t>
-    </r>
   </si>
   <si>
     <t>WaveletsV2 (Coiflet2,  4 Level, T 1s) Var, Sub, Entr</t>
@@ -342,15 +305,18 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>Coiflet2 Wavelet w/4 levels, T2 second, Variance, Subbands, and entropy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,19 +467,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)_x0000_"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1228,23 +1181,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J240"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J252"/>
   <sheetViews>
-    <sheetView topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C235" sqref="C235"/>
+    <sheetView tabSelected="1" topLeftCell="A227" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.59765625" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" style="1"/>
-    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1302,7 +1255,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1331,7 +1284,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1360,7 +1313,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1377,7 +1330,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1406,7 +1359,7 @@
         <v>782.77</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1423,7 +1376,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1440,7 +1393,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1457,7 +1410,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1474,7 +1427,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1491,7 +1444,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1508,7 +1461,7 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1525,7 +1478,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1542,7 +1495,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1559,7 +1512,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1576,7 +1529,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1593,7 +1546,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1610,7 +1563,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1627,7 +1580,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1644,7 +1597,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1673,7 +1626,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1690,7 +1643,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1707,7 +1660,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1724,7 +1677,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1741,7 +1694,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1758,7 +1711,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1775,7 +1728,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1792,7 +1745,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1809,7 +1762,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1826,7 +1779,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1843,7 +1796,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1860,7 +1813,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1889,7 +1842,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -1906,7 +1859,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1923,7 +1876,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1940,7 +1893,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1957,7 +1910,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -1974,7 +1927,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1991,7 +1944,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -2008,7 +1961,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -2025,7 +1978,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2042,7 +1995,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -2059,7 +2012,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -2076,7 +2029,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -2105,7 +2058,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -2122,7 +2075,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -2139,7 +2092,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -2156,7 +2109,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -2173,7 +2126,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2190,7 +2143,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2207,7 +2160,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -2224,7 +2177,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -2241,7 +2194,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -2258,7 +2211,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>27</v>
       </c>
@@ -2275,7 +2228,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -2292,7 +2245,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -2321,7 +2274,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -2338,7 +2291,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -2355,7 +2308,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>31</v>
       </c>
@@ -2372,7 +2325,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -2392,7 +2345,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -2409,7 +2362,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -2426,7 +2379,7 @@
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2443,7 +2396,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>20</v>
       </c>
@@ -2460,7 +2413,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -2477,7 +2430,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -2506,7 +2459,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>27</v>
       </c>
@@ -2523,7 +2476,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -2540,7 +2493,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>29</v>
       </c>
@@ -2557,7 +2510,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -2574,7 +2527,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>30</v>
       </c>
@@ -2591,7 +2544,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>31</v>
       </c>
@@ -2608,7 +2561,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -2625,7 +2578,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -2642,7 +2595,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2659,7 +2612,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -2676,7 +2629,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -2693,7 +2646,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -2722,7 +2675,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -2739,7 +2692,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -2756,7 +2709,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>29</v>
       </c>
@@ -2773,7 +2726,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -2790,7 +2743,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -2807,7 +2760,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>31</v>
       </c>
@@ -2824,7 +2777,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -2841,7 +2794,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -2858,7 +2811,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -2875,7 +2828,7 @@
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -2892,7 +2845,7 @@
         <v>0.72699999999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>23</v>
       </c>
@@ -2909,7 +2862,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>26</v>
       </c>
@@ -2938,7 +2891,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>27</v>
       </c>
@@ -2955,7 +2908,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>28</v>
       </c>
@@ -2972,7 +2925,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>29</v>
       </c>
@@ -2989,7 +2942,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -3006,7 +2959,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>30</v>
       </c>
@@ -3023,7 +2976,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>31</v>
       </c>
@@ -3040,7 +2993,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -3057,7 +3010,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -3074,7 +3027,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>19</v>
       </c>
@@ -3091,7 +3044,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -3108,7 +3061,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>23</v>
       </c>
@@ -3125,7 +3078,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>26</v>
       </c>
@@ -3142,7 +3095,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>27</v>
       </c>
@@ -3159,7 +3112,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>28</v>
       </c>
@@ -3176,7 +3129,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>29</v>
       </c>
@@ -3193,7 +3146,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -3210,7 +3163,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -3227,7 +3180,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>31</v>
       </c>
@@ -3244,7 +3197,7 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>15</v>
       </c>
@@ -3261,7 +3214,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -3278,7 +3231,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>19</v>
       </c>
@@ -3295,7 +3248,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>20</v>
       </c>
@@ -3312,7 +3265,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>23</v>
       </c>
@@ -3329,7 +3282,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>26</v>
       </c>
@@ -3346,7 +3299,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>27</v>
       </c>
@@ -3363,7 +3316,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>28</v>
       </c>
@@ -3380,7 +3333,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>29</v>
       </c>
@@ -3409,7 +3362,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>22</v>
       </c>
@@ -3426,7 +3379,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>30</v>
       </c>
@@ -3443,7 +3396,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>31</v>
       </c>
@@ -3460,7 +3413,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>15</v>
       </c>
@@ -3477,7 +3430,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -3494,7 +3447,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>19</v>
       </c>
@@ -3511,7 +3464,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>20</v>
       </c>
@@ -3528,7 +3481,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>23</v>
       </c>
@@ -3545,7 +3498,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -3562,7 +3515,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>27</v>
       </c>
@@ -3579,7 +3532,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>28</v>
       </c>
@@ -3596,7 +3549,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>29</v>
       </c>
@@ -3613,7 +3566,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>22</v>
       </c>
@@ -3630,7 +3583,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>30</v>
       </c>
@@ -3659,7 +3612,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>31</v>
       </c>
@@ -3676,7 +3629,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>15</v>
       </c>
@@ -3693,7 +3646,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>18</v>
       </c>
@@ -3710,7 +3663,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>19</v>
       </c>
@@ -3727,7 +3680,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>20</v>
       </c>
@@ -3744,7 +3697,7 @@
         <v>0.73299999999999998</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>23</v>
       </c>
@@ -3761,7 +3714,7 @@
         <v>0.82099999999999995</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>26</v>
       </c>
@@ -3778,7 +3731,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>27</v>
       </c>
@@ -3795,7 +3748,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>28</v>
       </c>
@@ -3812,7 +3765,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>29</v>
       </c>
@@ -3841,7 +3794,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>22</v>
       </c>
@@ -3858,7 +3811,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>30</v>
       </c>
@@ -3875,7 +3828,7 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>31</v>
       </c>
@@ -3892,7 +3845,7 @@
         <v>0.79900000000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>15</v>
       </c>
@@ -3909,7 +3862,7 @@
         <v>0.80700000000000005</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>18</v>
       </c>
@@ -3926,7 +3879,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>19</v>
       </c>
@@ -3943,7 +3896,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>20</v>
       </c>
@@ -3960,7 +3913,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>23</v>
       </c>
@@ -3977,7 +3930,7 @@
         <v>0.84799999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>26</v>
       </c>
@@ -3994,7 +3947,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>27</v>
       </c>
@@ -4011,7 +3964,7 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>28</v>
       </c>
@@ -4028,7 +3981,7 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>29</v>
       </c>
@@ -4057,7 +4010,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>22</v>
       </c>
@@ -4074,7 +4027,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>30</v>
       </c>
@@ -4091,7 +4044,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>31</v>
       </c>
@@ -4108,7 +4061,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>15</v>
       </c>
@@ -4125,7 +4078,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>18</v>
       </c>
@@ -4142,7 +4095,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>19</v>
       </c>
@@ -4159,7 +4112,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>20</v>
       </c>
@@ -4176,7 +4129,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>23</v>
       </c>
@@ -4193,7 +4146,7 @@
         <v>0.82299999999999995</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>26</v>
       </c>
@@ -4210,7 +4163,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>27</v>
       </c>
@@ -4227,7 +4180,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>28</v>
       </c>
@@ -4244,7 +4197,7 @@
         <v>0.89400000000000002</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>29</v>
       </c>
@@ -4273,7 +4226,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>22</v>
       </c>
@@ -4290,7 +4243,7 @@
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>30</v>
       </c>
@@ -4307,7 +4260,7 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>31</v>
       </c>
@@ -4324,7 +4277,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>75</v>
       </c>
@@ -4353,7 +4306,7 @@
         <v>1716</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>75</v>
       </c>
@@ -4382,7 +4335,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>75</v>
       </c>
@@ -4411,7 +4364,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>75</v>
       </c>
@@ -4440,7 +4393,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>75</v>
       </c>
@@ -4469,7 +4422,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>71</v>
       </c>
@@ -4486,12 +4439,12 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="15.75">
+    <row r="194" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>15</v>
       </c>
@@ -4508,7 +4461,7 @@
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>18</v>
       </c>
@@ -4525,7 +4478,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>19</v>
       </c>
@@ -4542,7 +4495,7 @@
         <v>0.86499999999999999</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>20</v>
       </c>
@@ -4559,7 +4512,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>23</v>
       </c>
@@ -4576,7 +4529,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>26</v>
       </c>
@@ -4593,7 +4546,7 @@
         <v>0.91900000000000004</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>27</v>
       </c>
@@ -4610,7 +4563,7 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>28</v>
       </c>
@@ -4627,7 +4580,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>29</v>
       </c>
@@ -4644,7 +4597,7 @@
         <v>0.51600000000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>22</v>
       </c>
@@ -4661,7 +4614,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>30</v>
       </c>
@@ -4678,7 +4631,7 @@
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>31</v>
       </c>
@@ -4695,7 +4648,7 @@
         <v>0.66100000000000003</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>61</v>
       </c>
@@ -4712,15 +4665,15 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C208" s="6"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75">
+    <row r="209" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>15</v>
       </c>
@@ -4737,7 +4690,7 @@
         <v>0.64400000000000002</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>18</v>
       </c>
@@ -4754,7 +4707,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>19</v>
       </c>
@@ -4771,7 +4724,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>20</v>
       </c>
@@ -4788,7 +4741,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>23</v>
       </c>
@@ -4805,7 +4758,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>26</v>
       </c>
@@ -4822,7 +4775,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>27</v>
       </c>
@@ -4839,7 +4792,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>28</v>
       </c>
@@ -4856,7 +4809,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>29</v>
       </c>
@@ -4873,7 +4826,7 @@
         <v>0.51400000000000001</v>
       </c>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>22</v>
       </c>
@@ -4890,7 +4843,7 @@
         <v>0.81499999999999995</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>30</v>
       </c>
@@ -4907,7 +4860,7 @@
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>31</v>
       </c>
@@ -4924,7 +4877,7 @@
         <v>0.66100000000000003</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>61</v>
       </c>
@@ -4941,15 +4894,15 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="223" spans="1:5">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C223" s="6"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75">
+    <row r="224" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>15</v>
       </c>
@@ -4957,7 +4910,7 @@
         <v>16</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D225" t="s">
         <v>83</v>
@@ -4966,7 +4919,7 @@
         <v>0.71599999999999997</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>18</v>
       </c>
@@ -4974,7 +4927,7 @@
         <v>16</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D226" t="s">
         <v>83</v>
@@ -4983,7 +4936,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>19</v>
       </c>
@@ -4991,7 +4944,7 @@
         <v>16</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D227" t="s">
         <v>83</v>
@@ -5000,7 +4953,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>20</v>
       </c>
@@ -5008,7 +4961,7 @@
         <v>16</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D228" t="s">
         <v>83</v>
@@ -5017,7 +4970,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>23</v>
       </c>
@@ -5025,7 +4978,7 @@
         <v>16</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D229" t="s">
         <v>83</v>
@@ -5034,7 +4987,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>26</v>
       </c>
@@ -5042,7 +4995,7 @@
         <v>16</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D230" t="s">
         <v>83</v>
@@ -5051,7 +5004,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>27</v>
       </c>
@@ -5059,7 +5012,7 @@
         <v>16</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D231" t="s">
         <v>83</v>
@@ -5068,7 +5021,7 @@
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>28</v>
       </c>
@@ -5076,7 +5029,7 @@
         <v>16</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D232" t="s">
         <v>83</v>
@@ -5085,7 +5038,7 @@
         <v>0.57099999999999995</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>29</v>
       </c>
@@ -5093,7 +5046,7 @@
         <v>16</v>
       </c>
       <c r="C233" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D233" t="s">
         <v>83</v>
@@ -5102,7 +5055,7 @@
         <v>0.499</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>22</v>
       </c>
@@ -5110,7 +5063,7 @@
         <v>16</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D234" t="s">
         <v>83</v>
@@ -5119,7 +5072,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>30</v>
       </c>
@@ -5127,7 +5080,7 @@
         <v>16</v>
       </c>
       <c r="C235" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D235" t="s">
         <v>83</v>
@@ -5136,7 +5089,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>31</v>
       </c>
@@ -5144,7 +5097,7 @@
         <v>16</v>
       </c>
       <c r="C236" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D236" t="s">
         <v>83</v>
@@ -5153,7 +5106,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>61</v>
       </c>
@@ -5161,7 +5114,7 @@
         <v>16</v>
       </c>
       <c r="C237" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D237" t="s">
         <v>83</v>
@@ -5170,14 +5123,230 @@
         <v>0.54100000000000004</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="15.75">
+    <row r="239" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A239" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" ht="15.75">
-      <c r="A240" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>15</v>
+      </c>
+      <c r="B240" t="s">
+        <v>16</v>
+      </c>
+      <c r="C240" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D240" t="s">
+        <v>83</v>
+      </c>
+      <c r="E240" s="1">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>18</v>
+      </c>
+      <c r="B241" t="s">
+        <v>16</v>
+      </c>
+      <c r="C241" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D241" t="s">
+        <v>83</v>
+      </c>
+      <c r="E241" s="1">
+        <v>0.90200000000000002</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>19</v>
+      </c>
+      <c r="B242" t="s">
+        <v>16</v>
+      </c>
+      <c r="C242" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D242" t="s">
+        <v>83</v>
+      </c>
+      <c r="E242" s="1">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>20</v>
+      </c>
+      <c r="B243" t="s">
+        <v>16</v>
+      </c>
+      <c r="C243" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D243" t="s">
+        <v>83</v>
+      </c>
+      <c r="E243" s="1">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>23</v>
+      </c>
+      <c r="B244" t="s">
+        <v>16</v>
+      </c>
+      <c r="C244" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D244" t="s">
+        <v>83</v>
+      </c>
+      <c r="E244" s="1">
+        <v>0.89700000000000002</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>26</v>
+      </c>
+      <c r="B245" t="s">
+        <v>16</v>
+      </c>
+      <c r="C245" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D245" t="s">
+        <v>83</v>
+      </c>
+      <c r="E245" s="1">
+        <v>0.92600000000000005</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>27</v>
+      </c>
+      <c r="B246" t="s">
+        <v>16</v>
+      </c>
+      <c r="C246" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D246" t="s">
+        <v>83</v>
+      </c>
+      <c r="E246" s="1">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>28</v>
+      </c>
+      <c r="B247" t="s">
+        <v>16</v>
+      </c>
+      <c r="C247" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D247" t="s">
+        <v>83</v>
+      </c>
+      <c r="E247" s="1">
+        <v>0.82899999999999996</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>29</v>
+      </c>
+      <c r="B248" t="s">
+        <v>16</v>
+      </c>
+      <c r="C248" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D248" t="s">
+        <v>83</v>
+      </c>
+      <c r="E248" s="1">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>22</v>
+      </c>
+      <c r="B249" t="s">
+        <v>16</v>
+      </c>
+      <c r="C249" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D249" t="s">
+        <v>83</v>
+      </c>
+      <c r="E249" s="1">
+        <v>0.81399999999999995</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>30</v>
+      </c>
+      <c r="B250" t="s">
+        <v>16</v>
+      </c>
+      <c r="C250" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D250" t="s">
+        <v>83</v>
+      </c>
+      <c r="E250" s="1">
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>31</v>
+      </c>
+      <c r="B251" t="s">
+        <v>16</v>
+      </c>
+      <c r="C251" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D251" t="s">
+        <v>83</v>
+      </c>
+      <c r="E251" s="1">
+        <v>0.73499999999999999</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>61</v>
+      </c>
+      <c r="B252" t="s">
+        <v>16</v>
+      </c>
+      <c r="C252" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D252" t="s">
+        <v>83</v>
+      </c>
+      <c r="E252" s="1">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -5187,23 +5356,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="10.796875" customWidth="1"/>
+    <col min="2" max="16" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="42.75">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -5253,7 +5422,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -5298,7 +5467,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -5345,7 +5514,7 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -5390,7 +5559,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5439,7 +5608,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -5484,7 +5653,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -5531,7 +5700,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -5576,7 +5745,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -5623,7 +5792,7 @@
         <v>0.77400000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5668,7 +5837,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -5715,7 +5884,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -5744,7 +5913,7 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -5773,7 +5942,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -5820,7 +5989,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -5867,7 +6036,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -5914,7 +6083,7 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5959,7 +6128,7 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -6004,7 +6173,7 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -6049,9 +6218,9 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1">
         <v>0.64100000000000001</v>
@@ -6098,9 +6267,9 @@
       </c>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1">
         <v>0.64400000000000002</v>
@@ -6145,9 +6314,9 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="1">
         <v>0.71599999999999997</v>
@@ -6192,27 +6361,27 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>15</v>
       </c>
@@ -6253,7 +6422,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>

</xml_diff>

<commit_message>
added lstm for the 2 s wavelet packet features
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_3F0B10B738445A2349E55591072AFD6EEF2C4A61" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{2D939E17-2C9A-402C-8FB0-D8CD806C28BB}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_3F0B10B738445A2349E55591072AFD6EEF2C4A61" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FCF857E5-3278-4A30-AEBB-8830F2DA8E2F}"/>
   <bookViews>
     <workbookView xWindow="3204" yWindow="456" windowWidth="21996" windowHeight="13380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="89">
   <si>
     <t>ModelType</t>
   </si>
@@ -1186,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J252"/>
+  <dimension ref="A1:J253"/>
   <sheetViews>
-    <sheetView topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A252" sqref="A252"/>
+    <sheetView topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G259" sqref="G259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5353,6 +5353,23 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>71</v>
+      </c>
+      <c r="B253" t="s">
+        <v>72</v>
+      </c>
+      <c r="C253" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D253" t="s">
+        <v>83</v>
+      </c>
+      <c r="E253" s="1">
+        <v>0.72099999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5367,7 +5384,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6315,7 +6332,9 @@
         <v>0.7</v>
       </c>
       <c r="O21" s="1"/>
-      <c r="P21" s="4"/>
+      <c r="P21" s="4">
+        <v>0.72099999999999997</v>
+      </c>
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added coiflet2 with 2-level transform results
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="700" windowWidth="22000" windowHeight="13380" activeTab="1"/>
+    <workbookView xWindow="7840" yWindow="760" windowWidth="19080" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="97">
   <si>
     <t>ModelType</t>
   </si>
@@ -323,6 +323,62 @@
   <si>
     <t>WaveletsV2(Haar, 4 Level, T 1s) Var,Sub,Entr</t>
   </si>
+  <si>
+    <t>Coiflet2 Wavelet w/2 levels, T2 second, Variance, Entropy, No subbands (as that only considers levels &gt; 2) (Total 7 Features)</t>
+  </si>
+  <si>
+    <t>FeaturesWavelets_coif2_Lvl2_T2.mat</t>
+  </si>
+  <si>
+    <t>WaveletsV2 (Coiflet2,  2 Level, T 2s)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WaveletsV2 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[7 Features]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Coiflet2, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Levels, T2s)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -331,7 +387,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +533,15 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -825,7 +890,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -835,6 +900,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -880,7 +948,19 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1197,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J269"/>
+  <dimension ref="A1:J283"/>
   <sheetViews>
-    <sheetView topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E256" sqref="E256:E268"/>
+    <sheetView topLeftCell="A261" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E271" sqref="E271:E283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5610,6 +5690,232 @@
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C269" s="6"/>
     </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A270" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>15</v>
+      </c>
+      <c r="B271" t="s">
+        <v>16</v>
+      </c>
+      <c r="C271" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D271" t="s">
+        <v>94</v>
+      </c>
+      <c r="E271" s="1">
+        <v>0.70099999999999996</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>18</v>
+      </c>
+      <c r="B272" t="s">
+        <v>16</v>
+      </c>
+      <c r="C272" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D272" t="s">
+        <v>94</v>
+      </c>
+      <c r="E272" s="1">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>19</v>
+      </c>
+      <c r="B273" t="s">
+        <v>16</v>
+      </c>
+      <c r="C273" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D273" t="s">
+        <v>94</v>
+      </c>
+      <c r="E273" s="1">
+        <v>0.84599999999999997</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>20</v>
+      </c>
+      <c r="B274" t="s">
+        <v>16</v>
+      </c>
+      <c r="C274" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D274" t="s">
+        <v>94</v>
+      </c>
+      <c r="E274" s="1">
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>23</v>
+      </c>
+      <c r="B275" t="s">
+        <v>16</v>
+      </c>
+      <c r="C275" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D275" t="s">
+        <v>94</v>
+      </c>
+      <c r="E275" s="1">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>26</v>
+      </c>
+      <c r="B276" t="s">
+        <v>16</v>
+      </c>
+      <c r="C276" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D276" t="s">
+        <v>94</v>
+      </c>
+      <c r="E276" s="1">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>27</v>
+      </c>
+      <c r="B277" t="s">
+        <v>16</v>
+      </c>
+      <c r="C277" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D277" t="s">
+        <v>94</v>
+      </c>
+      <c r="E277" s="1">
+        <v>0.68799999999999994</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>28</v>
+      </c>
+      <c r="B278" t="s">
+        <v>16</v>
+      </c>
+      <c r="C278" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D278" t="s">
+        <v>94</v>
+      </c>
+      <c r="E278" s="1">
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>29</v>
+      </c>
+      <c r="B279" t="s">
+        <v>16</v>
+      </c>
+      <c r="C279" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D279" t="s">
+        <v>94</v>
+      </c>
+      <c r="E279" s="1">
+        <v>0.53900000000000003</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>22</v>
+      </c>
+      <c r="B280" t="s">
+        <v>16</v>
+      </c>
+      <c r="C280" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D280" t="s">
+        <v>94</v>
+      </c>
+      <c r="E280" s="1">
+        <v>0.77700000000000002</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>30</v>
+      </c>
+      <c r="B281" t="s">
+        <v>16</v>
+      </c>
+      <c r="C281" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D281" t="s">
+        <v>94</v>
+      </c>
+      <c r="E281" s="1">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>31</v>
+      </c>
+      <c r="B282" t="s">
+        <v>16</v>
+      </c>
+      <c r="C282" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D282" t="s">
+        <v>94</v>
+      </c>
+      <c r="E282" s="1">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>61</v>
+      </c>
+      <c r="B283" t="s">
+        <v>16</v>
+      </c>
+      <c r="C283" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D283" t="s">
+        <v>94</v>
+      </c>
+      <c r="E283" s="1">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5621,10 +5927,10 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6719,7 +7025,51 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
+      <c r="A25" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
@@ -6758,8 +7108,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q24">
-    <cfRule type="top10" dxfId="0" priority="7" percent="1" rank="3"/>
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="top10" dxfId="1" priority="9" percent="1" rank="3"/>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:Q25">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
added LSTM and NN for waveletV2-coifletT2
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="760" windowWidth="19080" windowHeight="13380" activeTab="1"/>
+    <workbookView xWindow="1400" yWindow="760" windowWidth="24200" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -948,19 +948,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -5926,11 +5914,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6879,9 +6867,11 @@
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="4">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="Q21" s="1"/>
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0.88100000000000001</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
@@ -7108,7 +7098,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q24">
-    <cfRule type="top10" dxfId="1" priority="9" percent="1" rank="3"/>
+    <cfRule type="top10" dxfId="0" priority="9" percent="1" rank="3"/>
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added result for Hampel filtered Wavelet2
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="760" windowWidth="24200" windowHeight="13380" activeTab="1"/>
+    <workbookView xWindow="2440" yWindow="720" windowWidth="21720" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="98">
   <si>
     <t>ModelType</t>
   </si>
@@ -378,6 +378,9 @@
       </rPr>
       <t xml:space="preserve"> Levels, T2s)</t>
     </r>
+  </si>
+  <si>
+    <t>WaveletsV2 (Coiflet2,  4 Level, T 2s) with Hampel Filter</t>
   </si>
 </sst>
 </file>
@@ -5912,13 +5915,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6875,93 +6878,95 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B22" s="1">
-        <v>0.64400000000000002</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="C22" s="1">
-        <v>0.90100000000000002</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="D22" s="1">
-        <v>0.86</v>
+        <v>0.875</v>
       </c>
       <c r="E22" s="1">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="L22" s="1">
         <v>0.81100000000000005</v>
       </c>
-      <c r="F22" s="1">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0.77600000000000002</v>
-      </c>
       <c r="M22" s="1">
-        <v>0.66100000000000003</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="N22" s="1">
-        <v>0.71099999999999997</v>
+        <v>0.81299999999999994</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="1">
+        <v>0.93899999999999995</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1">
-        <v>0.53800000000000003</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="C23" s="1">
-        <v>0.77</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="D23" s="1">
-        <v>0.73099999999999998</v>
+        <v>0.86</v>
       </c>
       <c r="E23" s="1">
-        <v>0.68700000000000006</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="F23" s="1">
-        <v>0.76400000000000001</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="G23" s="1">
-        <v>0.80500000000000005</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="H23" s="1">
-        <v>0.71499999999999997</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="I23" s="1">
-        <v>0.76400000000000001</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="J23" s="1">
-        <v>0.58699999999999997</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="K23" s="1">
-        <v>0.76100000000000001</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="L23" s="1">
-        <v>0.73899999999999999</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="M23" s="1">
-        <v>0.70399999999999996</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="N23" s="1">
-        <v>0.67100000000000004</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -6969,135 +6974,182 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B24" s="1">
-        <v>0.71599999999999997</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="C24" s="1">
-        <v>0.90600000000000003</v>
+        <v>0.77</v>
       </c>
       <c r="D24" s="1">
-        <v>0.85699999999999998</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="E24" s="1">
-        <v>0.81599999999999995</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="F24" s="1">
-        <v>0.88300000000000001</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="G24" s="1">
-        <v>0.92100000000000004</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="H24" s="1">
-        <v>0.79200000000000004</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="I24" s="1">
-        <v>0.57099999999999995</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="J24" s="1">
-        <v>0.499</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="K24" s="1">
-        <v>0.76300000000000001</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="L24" s="1">
-        <v>0.67900000000000005</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="M24" s="1">
-        <v>0.61</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="N24" s="1">
-        <v>0.54100000000000004</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.499</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B26" s="3">
         <v>0.70099999999999996</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C26" s="3">
         <v>0.89</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D26" s="3">
         <v>0.84599999999999997</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E26" s="3">
         <v>0.78900000000000003</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F26" s="3">
         <v>0.88200000000000001</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G26" s="8">
         <v>0.92300000000000004</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H26" s="3">
         <v>0.68799999999999994</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I26" s="3">
         <v>0.71799999999999997</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J26" s="3">
         <v>0.53900000000000003</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K26" s="3">
         <v>0.77700000000000002</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L26" s="3">
         <v>0.74</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M26" s="3">
         <v>0.61499999999999999</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N26" s="3">
         <v>0.73699999999999999</v>
       </c>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:Q24">
+  <conditionalFormatting sqref="B2:Q25">
     <cfRule type="top10" dxfId="0" priority="9" percent="1" rank="3"/>
     <cfRule type="colorScale" priority="10">
       <colorScale>
@@ -7108,7 +7160,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:Q25">
+  <conditionalFormatting sqref="B2:Q26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Updated coiflet2 hampel to correct Lvl3 label
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todds\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulbirmiwal/Documents/UWMSDS/Capstone/EnvNoiseDetector/data/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_3F086AA34A84638E21E1772C784AEA49CDEA746B" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3507679D-A75E-44EC-82B3-02EC07897062}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19400" windowHeight="12200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
     <sheet name="Plot" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -380,9 +379,6 @@
     </r>
   </si>
   <si>
-    <t>WaveletsV2 (Coiflet2,  4 Level, T 2s) with Hampel Filter</t>
-  </si>
-  <si>
     <t>Model Performance for SNR 6 dB</t>
   </si>
   <si>
@@ -438,16 +434,19 @@
   </si>
   <si>
     <t>Block length (s)</t>
+  </si>
+  <si>
+    <t>WaveletsV2 (Coiflet2,  3 Level, T 2s) with Hampel Filter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1334,23 +1333,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J283"/>
   <sheetViews>
-    <sheetView topLeftCell="A261" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E271" sqref="E271:E283"/>
+    <sheetView topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B285" sqref="B285"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.73046875" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" style="1"/>
-    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1437,7 +1436,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1512,7 +1511,7 @@
         <v>782.77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1546,7 +1545,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1580,7 +1579,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1597,7 +1596,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1614,7 +1613,7 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>0.75800000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1665,7 +1664,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1681,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1716,7 +1715,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1796,7 +1795,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1847,7 +1846,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1932,7 +1931,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1995,7 +1994,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2012,7 +2011,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2063,7 +2062,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -2080,7 +2079,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -2114,7 +2113,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -2165,7 +2164,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -2245,7 +2244,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -2279,7 +2278,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2296,7 +2295,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -2330,7 +2329,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -2364,7 +2363,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>27</v>
       </c>
@@ -2381,7 +2380,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>31</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -2498,7 +2497,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -2532,7 +2531,7 @@
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>20</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>27</v>
       </c>
@@ -2629,7 +2628,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>29</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -2680,7 +2679,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>30</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>31</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -2799,7 +2798,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -2828,7 +2827,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>29</v>
       </c>
@@ -2879,7 +2878,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>31</v>
       </c>
@@ -2930,7 +2929,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -2981,7 +2980,7 @@
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -2998,7 +2997,7 @@
         <v>0.72699999999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>23</v>
       </c>
@@ -3015,7 +3014,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>26</v>
       </c>
@@ -3044,7 +3043,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>27</v>
       </c>
@@ -3061,7 +3060,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>28</v>
       </c>
@@ -3078,7 +3077,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>29</v>
       </c>
@@ -3095,7 +3094,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -3112,7 +3111,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>30</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>31</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -3163,7 +3162,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -3180,7 +3179,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>19</v>
       </c>
@@ -3197,7 +3196,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>23</v>
       </c>
@@ -3231,7 +3230,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>26</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>27</v>
       </c>
@@ -3265,7 +3264,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>28</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>29</v>
       </c>
@@ -3299,7 +3298,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>31</v>
       </c>
@@ -3350,7 +3349,7 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>15</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>19</v>
       </c>
@@ -3401,7 +3400,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>20</v>
       </c>
@@ -3418,7 +3417,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>23</v>
       </c>
@@ -3435,7 +3434,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>26</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>27</v>
       </c>
@@ -3469,7 +3468,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>28</v>
       </c>
@@ -3486,7 +3485,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9">
       <c r="A129" t="s">
         <v>29</v>
       </c>
@@ -3515,7 +3514,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9">
       <c r="A130" t="s">
         <v>22</v>
       </c>
@@ -3532,7 +3531,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9">
       <c r="A131" t="s">
         <v>30</v>
       </c>
@@ -3549,7 +3548,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9">
       <c r="A132" t="s">
         <v>31</v>
       </c>
@@ -3566,7 +3565,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9">
       <c r="A134" t="s">
         <v>15</v>
       </c>
@@ -3583,7 +3582,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9">
       <c r="A136" t="s">
         <v>19</v>
       </c>
@@ -3617,7 +3616,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9">
       <c r="A137" t="s">
         <v>20</v>
       </c>
@@ -3634,7 +3633,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9">
       <c r="A138" t="s">
         <v>23</v>
       </c>
@@ -3651,7 +3650,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -3668,7 +3667,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9">
       <c r="A140" t="s">
         <v>27</v>
       </c>
@@ -3685,7 +3684,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9">
       <c r="A141" t="s">
         <v>28</v>
       </c>
@@ -3702,7 +3701,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9">
       <c r="A142" t="s">
         <v>29</v>
       </c>
@@ -3719,7 +3718,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9">
       <c r="A143" t="s">
         <v>22</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9">
       <c r="A144" t="s">
         <v>30</v>
       </c>
@@ -3765,7 +3764,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>31</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9">
       <c r="A147" t="s">
         <v>15</v>
       </c>
@@ -3799,7 +3798,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9">
       <c r="A148" t="s">
         <v>18</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9">
       <c r="A149" t="s">
         <v>19</v>
       </c>
@@ -3833,7 +3832,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9">
       <c r="A150" t="s">
         <v>20</v>
       </c>
@@ -3850,7 +3849,7 @@
         <v>0.73299999999999998</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9">
       <c r="A151" t="s">
         <v>23</v>
       </c>
@@ -3867,7 +3866,7 @@
         <v>0.82099999999999995</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9">
       <c r="A152" t="s">
         <v>26</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9">
       <c r="A153" t="s">
         <v>27</v>
       </c>
@@ -3901,7 +3900,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9">
       <c r="A154" t="s">
         <v>28</v>
       </c>
@@ -3918,7 +3917,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9">
       <c r="A155" t="s">
         <v>29</v>
       </c>
@@ -3947,7 +3946,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9">
       <c r="A156" t="s">
         <v>22</v>
       </c>
@@ -3964,7 +3963,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9">
       <c r="A157" t="s">
         <v>30</v>
       </c>
@@ -3981,7 +3980,7 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9">
       <c r="A158" t="s">
         <v>31</v>
       </c>
@@ -3998,7 +3997,7 @@
         <v>0.79900000000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9">
       <c r="A160" t="s">
         <v>15</v>
       </c>
@@ -4015,7 +4014,7 @@
         <v>0.80700000000000005</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9">
       <c r="A161" t="s">
         <v>18</v>
       </c>
@@ -4032,7 +4031,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9">
       <c r="A162" t="s">
         <v>19</v>
       </c>
@@ -4049,7 +4048,7 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9">
       <c r="A163" t="s">
         <v>20</v>
       </c>
@@ -4066,7 +4065,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9">
       <c r="A164" t="s">
         <v>23</v>
       </c>
@@ -4083,7 +4082,7 @@
         <v>0.84799999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9">
       <c r="A165" t="s">
         <v>26</v>
       </c>
@@ -4100,7 +4099,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9">
       <c r="A166" t="s">
         <v>27</v>
       </c>
@@ -4117,7 +4116,7 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9">
       <c r="A167" t="s">
         <v>28</v>
       </c>
@@ -4134,7 +4133,7 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9">
       <c r="A168" t="s">
         <v>29</v>
       </c>
@@ -4163,7 +4162,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9">
       <c r="A169" t="s">
         <v>22</v>
       </c>
@@ -4180,7 +4179,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9">
       <c r="A170" t="s">
         <v>30</v>
       </c>
@@ -4197,7 +4196,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9">
       <c r="A171" t="s">
         <v>31</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9">
       <c r="A173" t="s">
         <v>15</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9">
       <c r="A174" t="s">
         <v>18</v>
       </c>
@@ -4248,7 +4247,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9">
       <c r="A175" t="s">
         <v>19</v>
       </c>
@@ -4265,7 +4264,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9">
       <c r="A176" t="s">
         <v>20</v>
       </c>
@@ -4282,7 +4281,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9">
       <c r="A177" t="s">
         <v>23</v>
       </c>
@@ -4299,7 +4298,7 @@
         <v>0.82299999999999995</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9">
       <c r="A178" t="s">
         <v>26</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9">
       <c r="A179" t="s">
         <v>27</v>
       </c>
@@ -4333,7 +4332,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9">
       <c r="A180" t="s">
         <v>28</v>
       </c>
@@ -4350,7 +4349,7 @@
         <v>0.89400000000000002</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9">
       <c r="A181" t="s">
         <v>29</v>
       </c>
@@ -4379,7 +4378,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9">
       <c r="A182" t="s">
         <v>22</v>
       </c>
@@ -4396,7 +4395,7 @@
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9">
       <c r="A183" t="s">
         <v>30</v>
       </c>
@@ -4413,7 +4412,7 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9">
       <c r="A184" t="s">
         <v>31</v>
       </c>
@@ -4430,7 +4429,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9">
       <c r="A186" t="s">
         <v>72</v>
       </c>
@@ -4459,7 +4458,7 @@
         <v>1716</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9">
       <c r="A187" t="s">
         <v>72</v>
       </c>
@@ -4488,7 +4487,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9">
       <c r="A188" t="s">
         <v>72</v>
       </c>
@@ -4517,7 +4516,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9">
       <c r="A189" t="s">
         <v>72</v>
       </c>
@@ -4546,7 +4545,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9">
       <c r="A190" t="s">
         <v>72</v>
       </c>
@@ -4575,7 +4574,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9">
       <c r="A192" t="s">
         <v>69</v>
       </c>
@@ -4592,12 +4591,12 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="194" spans="1:5" ht="16">
       <c r="A194" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
         <v>15</v>
       </c>
@@ -4614,7 +4613,7 @@
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
         <v>18</v>
       </c>
@@ -4631,7 +4630,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
         <v>19</v>
       </c>
@@ -4648,7 +4647,7 @@
         <v>0.86499999999999999</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
         <v>20</v>
       </c>
@@ -4665,7 +4664,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
         <v>23</v>
       </c>
@@ -4682,7 +4681,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
         <v>26</v>
       </c>
@@ -4699,7 +4698,7 @@
         <v>0.91900000000000004</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:5">
       <c r="A201" t="s">
         <v>27</v>
       </c>
@@ -4716,7 +4715,7 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:5">
       <c r="A202" t="s">
         <v>28</v>
       </c>
@@ -4733,7 +4732,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:5">
       <c r="A203" t="s">
         <v>29</v>
       </c>
@@ -4750,7 +4749,7 @@
         <v>0.51600000000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
         <v>22</v>
       </c>
@@ -4767,7 +4766,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
         <v>30</v>
       </c>
@@ -4784,7 +4783,7 @@
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:5">
       <c r="A206" t="s">
         <v>31</v>
       </c>
@@ -4801,7 +4800,7 @@
         <v>0.66100000000000003</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:5">
       <c r="A207" t="s">
         <v>60</v>
       </c>
@@ -4818,15 +4817,15 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:5">
       <c r="C208" s="5"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="209" spans="1:5" ht="16">
       <c r="A209" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
         <v>15</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>0.64400000000000002</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
         <v>18</v>
       </c>
@@ -4860,7 +4859,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
         <v>19</v>
       </c>
@@ -4877,7 +4876,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:5">
       <c r="A213" t="s">
         <v>20</v>
       </c>
@@ -4894,7 +4893,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
         <v>23</v>
       </c>
@@ -4911,7 +4910,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
         <v>26</v>
       </c>
@@ -4928,7 +4927,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>27</v>
       </c>
@@ -4945,7 +4944,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>28</v>
       </c>
@@ -4962,7 +4961,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
         <v>29</v>
       </c>
@@ -4979,7 +4978,7 @@
         <v>0.51400000000000001</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>22</v>
       </c>
@@ -4996,7 +4995,7 @@
         <v>0.81499999999999995</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
         <v>30</v>
       </c>
@@ -5013,7 +5012,7 @@
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>31</v>
       </c>
@@ -5030,7 +5029,7 @@
         <v>0.66100000000000003</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
         <v>60</v>
       </c>
@@ -5047,15 +5046,15 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:5">
       <c r="C223" s="5"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="224" spans="1:5" ht="16">
       <c r="A224" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:5">
       <c r="A225" t="s">
         <v>15</v>
       </c>
@@ -5072,7 +5071,7 @@
         <v>0.71599999999999997</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:5">
       <c r="A226" t="s">
         <v>18</v>
       </c>
@@ -5089,7 +5088,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:5">
       <c r="A227" t="s">
         <v>19</v>
       </c>
@@ -5106,7 +5105,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:5">
       <c r="A228" t="s">
         <v>20</v>
       </c>
@@ -5123,7 +5122,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:5">
       <c r="A229" t="s">
         <v>23</v>
       </c>
@@ -5140,7 +5139,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:5">
       <c r="A230" t="s">
         <v>26</v>
       </c>
@@ -5157,7 +5156,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:5">
       <c r="A231" t="s">
         <v>27</v>
       </c>
@@ -5174,7 +5173,7 @@
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:5">
       <c r="A232" t="s">
         <v>28</v>
       </c>
@@ -5191,7 +5190,7 @@
         <v>0.57099999999999995</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:5">
       <c r="A233" t="s">
         <v>29</v>
       </c>
@@ -5208,7 +5207,7 @@
         <v>0.499</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:5">
       <c r="A234" t="s">
         <v>22</v>
       </c>
@@ -5225,7 +5224,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:5">
       <c r="A235" t="s">
         <v>30</v>
       </c>
@@ -5242,7 +5241,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:5">
       <c r="A236" t="s">
         <v>31</v>
       </c>
@@ -5259,7 +5258,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:5">
       <c r="A237" t="s">
         <v>60</v>
       </c>
@@ -5276,12 +5275,12 @@
         <v>0.54100000000000004</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="239" spans="1:5" ht="16">
       <c r="A239" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:5">
       <c r="A240" t="s">
         <v>15</v>
       </c>
@@ -5298,7 +5297,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
         <v>18</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>0.90200000000000002</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>19</v>
       </c>
@@ -5332,7 +5331,7 @@
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:5">
       <c r="A243" t="s">
         <v>20</v>
       </c>
@@ -5349,7 +5348,7 @@
         <v>0.80700000000000005</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:5">
       <c r="A244" t="s">
         <v>23</v>
       </c>
@@ -5366,7 +5365,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:5">
       <c r="A245" t="s">
         <v>26</v>
       </c>
@@ -5383,7 +5382,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:5">
       <c r="A246" t="s">
         <v>27</v>
       </c>
@@ -5400,7 +5399,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:5">
       <c r="A247" t="s">
         <v>28</v>
       </c>
@@ -5417,7 +5416,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:5">
       <c r="A248" t="s">
         <v>29</v>
       </c>
@@ -5434,7 +5433,7 @@
         <v>0.60699999999999998</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:5">
       <c r="A249" t="s">
         <v>22</v>
       </c>
@@ -5451,7 +5450,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:5">
       <c r="A250" t="s">
         <v>30</v>
       </c>
@@ -5468,7 +5467,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:5">
       <c r="A251" t="s">
         <v>31</v>
       </c>
@@ -5485,7 +5484,7 @@
         <v>0.73499999999999999</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:5">
       <c r="A252" t="s">
         <v>60</v>
       </c>
@@ -5502,7 +5501,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:5">
       <c r="A253" t="s">
         <v>69</v>
       </c>
@@ -5519,12 +5518,12 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="255" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="255" spans="1:5" ht="16">
       <c r="A255" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:5">
       <c r="A256" t="s">
         <v>15</v>
       </c>
@@ -5541,7 +5540,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
         <v>18</v>
       </c>
@@ -5558,7 +5557,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>19</v>
       </c>
@@ -5575,7 +5574,7 @@
         <v>0.73099999999999998</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>20</v>
       </c>
@@ -5592,7 +5591,7 @@
         <v>0.68700000000000006</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>23</v>
       </c>
@@ -5609,7 +5608,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>26</v>
       </c>
@@ -5626,7 +5625,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>27</v>
       </c>
@@ -5643,7 +5642,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
         <v>28</v>
       </c>
@@ -5660,7 +5659,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
         <v>29</v>
       </c>
@@ -5677,7 +5676,7 @@
         <v>0.58699999999999997</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>22</v>
       </c>
@@ -5694,7 +5693,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:5">
       <c r="A266" t="s">
         <v>30</v>
       </c>
@@ -5711,7 +5710,7 @@
         <v>0.73899999999999999</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:5">
       <c r="A267" t="s">
         <v>31</v>
       </c>
@@ -5728,7 +5727,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>60</v>
       </c>
@@ -5745,15 +5744,15 @@
         <v>0.67100000000000004</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:5">
       <c r="C269" s="5"/>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:5">
       <c r="A270" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:5">
       <c r="A271" t="s">
         <v>15</v>
       </c>
@@ -5770,7 +5769,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:5">
       <c r="A272" t="s">
         <v>18</v>
       </c>
@@ -5787,7 +5786,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
         <v>19</v>
       </c>
@@ -5804,7 +5803,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
         <v>20</v>
       </c>
@@ -5821,7 +5820,7 @@
         <v>0.78900000000000003</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>23</v>
       </c>
@@ -5838,7 +5837,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>26</v>
       </c>
@@ -5855,7 +5854,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>27</v>
       </c>
@@ -5872,7 +5871,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>28</v>
       </c>
@@ -5889,7 +5888,7 @@
         <v>0.71799999999999997</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:5">
       <c r="A279" t="s">
         <v>29</v>
       </c>
@@ -5906,7 +5905,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>22</v>
       </c>
@@ -5923,7 +5922,7 @@
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
         <v>30</v>
       </c>
@@ -5940,7 +5939,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
         <v>31</v>
       </c>
@@ -5957,7 +5956,7 @@
         <v>0.61499999999999999</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:5">
       <c r="A283" t="s">
         <v>60</v>
       </c>
@@ -5981,32 +5980,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="16" width="10.86328125" customWidth="1"/>
-    <col min="18" max="19" width="10.86328125" customWidth="1"/>
+    <col min="4" max="16" width="10.83203125" customWidth="1"/>
+    <col min="18" max="19" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="45">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>15</v>
@@ -6057,9 +6056,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -6108,9 +6107,9 @@
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -6161,9 +6160,9 @@
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <v>26</v>
@@ -6212,9 +6211,9 @@
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <v>26</v>
@@ -6267,9 +6266,9 @@
         <v>0.61799999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6">
         <v>29</v>
@@ -6318,9 +6317,9 @@
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7">
         <v>29</v>
@@ -6371,9 +6370,9 @@
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -6422,9 +6421,9 @@
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -6475,9 +6474,9 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10">
         <v>13</v>
@@ -6526,9 +6525,9 @@
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -6579,9 +6578,9 @@
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12">
         <v>799</v>
@@ -6614,9 +6613,9 @@
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13">
         <v>200</v>
@@ -6649,7 +6648,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -6699,7 +6698,7 @@
       </c>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -6749,7 +6748,7 @@
       </c>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -6799,9 +6798,9 @@
       </c>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>500</v>
@@ -6850,9 +6849,9 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18">
         <v>500</v>
@@ -6901,9 +6900,9 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19">
         <v>500</v>
@@ -6952,7 +6951,7 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:19">
       <c r="A20" s="5" t="s">
         <v>81</v>
       </c>
@@ -7007,7 +7006,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:19">
       <c r="A21" s="5" t="s">
         <v>85</v>
       </c>
@@ -7064,9 +7063,9 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:19">
       <c r="A22" s="5" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -7116,7 +7115,7 @@
       <c r="R22" s="9"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19">
       <c r="A23" s="5" t="s">
         <v>82</v>
       </c>
@@ -7166,7 +7165,7 @@
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:19">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -7216,7 +7215,7 @@
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:19">
       <c r="A25" s="5" t="s">
         <v>83</v>
       </c>
@@ -7266,7 +7265,7 @@
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:19">
       <c r="A26" s="7" t="s">
         <v>93</v>
       </c>
@@ -7319,7 +7318,7 @@
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:19">
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -7337,27 +7336,27 @@
       <c r="R27" s="11"/>
       <c r="S27" s="11"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:19">
       <c r="D28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:19">
       <c r="D29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:19">
       <c r="D30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="4:16" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="4:16">
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>

</xml_diff>

<commit_message>
forgot to add BaggedTree result for 5lvl earlier
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -5996,7 +5996,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7089,7 +7089,9 @@
         <v>0.79300000000000004</v>
       </c>
       <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="9">
+        <v>0.94</v>
+      </c>
       <c r="J22" s="9">
         <v>0.82</v>
       </c>

</xml_diff>

<commit_message>
wavelet coeif2 lvl5 with hampel
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{9E768CC0-D6C1-4E0D-9020-C6F3EF599EDE}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{69AF0B5F-0620-4D15-8CB8-07FDEF9E8CF9}"/>
   <bookViews>
-    <workbookView xWindow="2112" yWindow="528" windowWidth="25980" windowHeight="14292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="756" windowWidth="20556" windowHeight="14292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="113">
   <si>
     <t>ModelType</t>
   </si>
@@ -327,9 +327,6 @@
     <t>Block length (s)</t>
   </si>
   <si>
-    <t>--</t>
-  </si>
-  <si>
     <t>* DWT = discrete wavelet transform</t>
   </si>
   <si>
@@ -369,12 +366,6 @@
     <t>DWT (Coiflet2, 4 levels)</t>
   </si>
   <si>
-    <t>DWT (Coiflet2, 5 levels,  Hampel Filter)</t>
-  </si>
-  <si>
-    <t>DWT (Coiflet2, 3 levels,  Hampel Filter)</t>
-  </si>
-  <si>
     <t>DWT (Debauchies4, 4 levels)</t>
   </si>
   <si>
@@ -385,6 +376,21 @@
   </si>
   <si>
     <t>DWT (Coiflet2, 2 levels)</t>
+  </si>
+  <si>
+    <t>DWT (Coiflet2, 5 levels)</t>
+  </si>
+  <si>
+    <t>DWT (Coiflet2, 5 levels, Hampel Filter)</t>
+  </si>
+  <si>
+    <t>DWT (Coiflet2, 3 levels, Hampel Filter)</t>
+  </si>
+  <si>
+    <t>95.9% (81.1%)</t>
+  </si>
+  <si>
+    <t>93.9% (81.4%)</t>
   </si>
 </sst>
 </file>
@@ -5961,13 +5967,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6040,7 +6046,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -6091,7 +6097,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -6144,7 +6150,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4">
         <v>26</v>
@@ -6195,7 +6201,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5">
         <v>26</v>
@@ -6250,7 +6256,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6">
         <v>29</v>
@@ -6301,7 +6307,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>29</v>
@@ -6354,7 +6360,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -6405,7 +6411,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -6458,7 +6464,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10">
         <v>13</v>
@@ -6509,7 +6515,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -6562,7 +6568,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12">
         <v>799</v>
@@ -6597,7 +6603,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13">
         <v>200</v>
@@ -6632,7 +6638,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14">
         <f>224*224*3</f>
@@ -6662,7 +6668,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15">
         <f>224*224*3</f>
@@ -6692,7 +6698,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16">
         <f>224*224*3</f>
@@ -6722,7 +6728,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17">
         <v>500</v>
@@ -6773,7 +6779,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18">
         <v>500</v>
@@ -6824,7 +6830,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19">
         <v>500</v>
@@ -6875,7 +6881,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20">
         <v>17</v>
@@ -6930,7 +6936,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21">
         <v>17</v>
@@ -6987,7 +6993,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B22">
         <v>49</v>
@@ -6996,159 +7002,157 @@
         <v>2</v>
       </c>
       <c r="D22" s="8">
-        <v>0.80400000000000005</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="E22" s="8">
         <v>0.91700000000000004</v>
       </c>
       <c r="F22" s="8">
-        <v>0.88700000000000001</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="G22" s="8">
         <v>0.79300000000000004</v>
       </c>
-      <c r="H22" s="8"/>
+      <c r="H22" s="8">
+        <v>0.92300000000000004</v>
+      </c>
       <c r="I22" s="8">
-        <v>0.94</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="J22" s="8">
-        <v>0.82</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="K22" s="8">
-        <v>0.879</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>91</v>
+        <v>0.88</v>
+      </c>
+      <c r="L22" s="8">
+        <v>0.90600000000000003</v>
       </c>
       <c r="M22" s="8">
-        <v>0.876</v>
+        <v>0.872</v>
       </c>
       <c r="N22" s="8">
-        <v>0.83799999999999997</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="O22" s="8">
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="P22" s="8">
-        <v>0.76500000000000001</v>
-      </c>
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="P22" s="8"/>
       <c r="Q22" s="8">
-        <v>0.95899999999999996</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="R22" s="8"/>
       <c r="S22" s="7"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C23" s="11">
         <v>2</v>
       </c>
       <c r="D23" s="8">
-        <v>0.67100000000000004</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="E23" s="8">
-        <v>0.89700000000000002</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="F23" s="8">
-        <v>0.875</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="G23" s="8">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="H23" s="8">
-        <v>0.89600000000000002</v>
-      </c>
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="H23" s="10"/>
       <c r="I23" s="8">
-        <v>0.92900000000000005</v>
+        <v>0.94</v>
       </c>
       <c r="J23" s="8">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="K23" s="8">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="L23" s="8">
-        <v>0.52</v>
-      </c>
+        <v>0.879</v>
+      </c>
+      <c r="L23" s="10"/>
       <c r="M23" s="8">
-        <v>0.85899999999999999</v>
+        <v>0.876</v>
       </c>
       <c r="N23" s="8">
-        <v>0.81100000000000005</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="O23" s="8">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="P23" s="8">
         <v>0.76500000000000001</v>
       </c>
-      <c r="P23" s="8">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>0.93899999999999995</v>
+      <c r="Q23" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="R23" s="8"/>
       <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C24" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="8">
-        <v>0.64400000000000002</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="E24" s="8">
-        <v>0.90100000000000002</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="F24" s="8">
-        <v>0.86</v>
+        <v>0.875</v>
       </c>
       <c r="G24" s="8">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="N24" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="H24" s="8">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="I24" s="8">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="J24" s="8">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="K24" s="8">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="L24" s="8">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="M24" s="8">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="N24" s="8">
-        <v>0.77600000000000002</v>
-      </c>
       <c r="O24" s="8">
-        <v>0.66100000000000003</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="P24" s="8">
-        <v>0.71099999999999997</v>
-      </c>
-      <c r="Q24" s="8"/>
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
+      <c r="S24" s="7"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25">
         <v>17</v>
@@ -7157,43 +7161,43 @@
         <v>1</v>
       </c>
       <c r="D25" s="8">
-        <v>0.53800000000000003</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="E25" s="8">
-        <v>0.77</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="F25" s="8">
-        <v>0.73099999999999998</v>
+        <v>0.86</v>
       </c>
       <c r="G25" s="8">
-        <v>0.68700000000000006</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="H25" s="8">
-        <v>0.76400000000000001</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="I25" s="8">
-        <v>0.80500000000000005</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="J25" s="8">
-        <v>0.71499999999999997</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="K25" s="8">
-        <v>0.76400000000000001</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="L25" s="8">
-        <v>0.58699999999999997</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="M25" s="8">
-        <v>0.76100000000000001</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="N25" s="8">
-        <v>0.73899999999999999</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="O25" s="8">
-        <v>0.70399999999999996</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="P25" s="8">
-        <v>0.67100000000000004</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -7201,52 +7205,52 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C26" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="8">
-        <v>0.71599999999999997</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="E26" s="8">
-        <v>0.90600000000000003</v>
+        <v>0.77</v>
       </c>
       <c r="F26" s="8">
-        <v>0.85699999999999998</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="G26" s="8">
-        <v>0.81599999999999995</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="H26" s="8">
-        <v>0.88300000000000001</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="I26" s="8">
-        <v>0.92100000000000004</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="J26" s="8">
-        <v>0.79200000000000004</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="K26" s="8">
-        <v>0.57099999999999995</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="L26" s="8">
-        <v>0.499</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="M26" s="8">
-        <v>0.76300000000000001</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="N26" s="8">
-        <v>0.67900000000000005</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="O26" s="8">
-        <v>0.61</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="P26" s="8">
-        <v>0.54100000000000004</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
@@ -7254,129 +7258,182 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C27" s="11">
         <v>2</v>
       </c>
       <c r="D27" s="8">
-        <v>0.70099999999999996</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="E27" s="8">
-        <v>0.89</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="F27" s="8">
-        <v>0.84599999999999997</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G27" s="8">
-        <v>0.78900000000000003</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="H27" s="8">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="I27" s="7">
-        <v>0.92300000000000004</v>
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.92100000000000004</v>
       </c>
       <c r="J27" s="8">
-        <v>0.68799999999999994</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="K27" s="8">
-        <v>0.71799999999999997</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="L27" s="8">
-        <v>0.53900000000000003</v>
+        <v>0.499</v>
       </c>
       <c r="M27" s="8">
-        <v>0.77700000000000002</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="N27" s="8">
-        <v>0.74</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="O27" s="8">
-        <v>0.61499999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="P27" s="8">
-        <v>0.73699999999999999</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
+      <c r="A28" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" s="11">
+        <v>2</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.89</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="G28" s="8">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="J28" s="8">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="K28" s="8">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="L28" s="8">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="M28" s="8">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="N28" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="O28" s="8">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="P28" s="8">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
-        <v>56</v>
-      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D36" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-    </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D36" t="s">
-        <v>99</v>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:S27">
+  <conditionalFormatting sqref="D2:S28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="90"/>

</xml_diff>

<commit_message>
fixed issues with wavelet coif2 lvl 4 t2
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{69AF0B5F-0620-4D15-8CB8-07FDEF9E8CF9}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{ACB52CEA-4607-43B5-B900-31107E24D4BB}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="756" windowWidth="20556" windowHeight="14292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1752" yWindow="324" windowWidth="26940" windowHeight="15732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="114">
   <si>
     <t>ModelType</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>93.9% (81.4%)</t>
+  </si>
+  <si>
+    <t>DWT (Coiflet2, 4 levels, Hampel Filter)</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1003,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -5967,13 +5976,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
+      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6939,52 +6948,50 @@
         <v>103</v>
       </c>
       <c r="B21">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C21" s="11">
         <v>2</v>
       </c>
       <c r="D21" s="8">
-        <v>0.65800000000000003</v>
+        <v>0.754</v>
       </c>
       <c r="E21" s="8">
-        <v>0.90200000000000002</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="F21" s="8">
-        <v>0.85199999999999998</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="G21" s="8">
-        <v>0.80700000000000005</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="H21" s="8">
-        <v>0.89700000000000002</v>
+        <v>0.91</v>
       </c>
       <c r="I21" s="8">
-        <v>0.92600000000000005</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="J21" s="8">
-        <v>0.78</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="K21" s="8">
-        <v>0.82899999999999996</v>
+        <v>0.873</v>
       </c>
       <c r="L21" s="8">
-        <v>0.60699999999999998</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="M21" s="8">
-        <v>0.81399999999999995</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="N21" s="8">
-        <v>0.78800000000000003</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="O21" s="8">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="P21" s="8">
-        <v>0.7</v>
-      </c>
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="P21" s="8"/>
       <c r="Q21" s="8">
-        <v>0.88100000000000001</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="R21" s="8"/>
       <c r="S21" s="7">
@@ -7097,115 +7104,115 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C24" s="11">
         <v>2</v>
       </c>
       <c r="D24" s="8">
-        <v>0.67100000000000004</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="E24" s="8">
-        <v>0.89700000000000002</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="F24" s="8">
-        <v>0.875</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="G24" s="8">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0.89600000000000002</v>
+        <v>0.8</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0.91100000000000003</v>
       </c>
       <c r="I24" s="8">
-        <v>0.92900000000000005</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="J24" s="8">
-        <v>0.79</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="K24" s="8">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="L24" s="8">
-        <v>0.52</v>
+        <v>0.879</v>
+      </c>
+      <c r="L24" s="10">
+        <v>0.90800000000000003</v>
       </c>
       <c r="M24" s="8">
-        <v>0.85899999999999999</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="N24" s="8">
-        <v>0.81100000000000005</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="O24" s="8">
-        <v>0.76500000000000001</v>
-      </c>
-      <c r="P24" s="8">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="Q24" s="8" t="s">
-        <v>112</v>
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8">
+        <v>0.83099999999999996</v>
       </c>
       <c r="R24" s="8"/>
       <c r="S24" s="7"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B25">
         <v>17</v>
       </c>
       <c r="C25" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="8">
-        <v>0.64400000000000002</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="E25" s="8">
-        <v>0.90100000000000002</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="F25" s="8">
-        <v>0.86</v>
+        <v>0.875</v>
       </c>
       <c r="G25" s="8">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="N25" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="H25" s="8">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="I25" s="8">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="J25" s="8">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="K25" s="8">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="L25" s="8">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="M25" s="8">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="N25" s="8">
-        <v>0.77600000000000002</v>
-      </c>
       <c r="O25" s="8">
-        <v>0.66100000000000003</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="P25" s="8">
-        <v>0.71099999999999997</v>
-      </c>
-      <c r="Q25" s="8"/>
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
+      <c r="S25" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26">
         <v>17</v>
@@ -7214,43 +7221,43 @@
         <v>1</v>
       </c>
       <c r="D26" s="8">
-        <v>0.53800000000000003</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="E26" s="8">
-        <v>0.77</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="F26" s="8">
-        <v>0.73099999999999998</v>
+        <v>0.86</v>
       </c>
       <c r="G26" s="8">
-        <v>0.68700000000000006</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="H26" s="8">
-        <v>0.76400000000000001</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="I26" s="8">
-        <v>0.80500000000000005</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="J26" s="8">
-        <v>0.71499999999999997</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="K26" s="8">
-        <v>0.76400000000000001</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="L26" s="8">
-        <v>0.58699999999999997</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="M26" s="8">
-        <v>0.76100000000000001</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="N26" s="8">
-        <v>0.73899999999999999</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="O26" s="8">
-        <v>0.70399999999999996</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="P26" s="8">
-        <v>0.67100000000000004</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
@@ -7258,52 +7265,52 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C27" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="8">
-        <v>0.71599999999999997</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="E27" s="8">
-        <v>0.90600000000000003</v>
+        <v>0.77</v>
       </c>
       <c r="F27" s="8">
-        <v>0.85699999999999998</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="G27" s="8">
-        <v>0.81599999999999995</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="H27" s="8">
-        <v>0.88300000000000001</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="I27" s="8">
-        <v>0.92100000000000004</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="J27" s="8">
-        <v>0.79200000000000004</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="K27" s="8">
-        <v>0.57099999999999995</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="L27" s="8">
-        <v>0.499</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="M27" s="8">
-        <v>0.76300000000000001</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="N27" s="8">
-        <v>0.67900000000000005</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="O27" s="8">
-        <v>0.61</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="P27" s="8">
-        <v>0.54100000000000004</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
@@ -7311,129 +7318,182 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C28" s="11">
         <v>2</v>
       </c>
       <c r="D28" s="8">
-        <v>0.70099999999999996</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="E28" s="8">
-        <v>0.89</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="F28" s="8">
-        <v>0.84599999999999997</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G28" s="8">
-        <v>0.78900000000000003</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="H28" s="8">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="I28" s="7">
-        <v>0.92300000000000004</v>
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0.92100000000000004</v>
       </c>
       <c r="J28" s="8">
-        <v>0.68799999999999994</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="K28" s="8">
-        <v>0.71799999999999997</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="L28" s="8">
-        <v>0.53900000000000003</v>
+        <v>0.499</v>
       </c>
       <c r="M28" s="8">
-        <v>0.77700000000000002</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="N28" s="8">
-        <v>0.74</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="O28" s="8">
-        <v>0.61499999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="P28" s="8">
-        <v>0.73699999999999999</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
+      <c r="A29" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29" s="11">
+        <v>2</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.89</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="G29" s="8">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="H29" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I29" s="7">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="K29" s="8">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="L29" s="8">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="M29" s="8">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="N29" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="O29" s="8">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="P29" s="8">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
-        <v>56</v>
-      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D36" s="3" t="s">
+    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D37" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D37" t="s">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:S28">
+  <conditionalFormatting sqref="D2:S29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="90"/>
@@ -7442,7 +7502,7 @@
         <color theme="7" tint="0.39997558519241921"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="76" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
redo on dwt level 4 no hampel
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{ACB52CEA-4607-43B5-B900-31107E24D4BB}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{07CBC4EF-469A-4221-ADA7-E18C4BAF1C7A}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="324" windowWidth="26940" windowHeight="15732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="876" windowWidth="26940" windowHeight="15732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -1003,13 +1003,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -6893,51 +6887,51 @@
         <v>103</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C20" s="11">
         <v>1</v>
       </c>
       <c r="D20" s="8">
-        <v>0.64100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="E20" s="8">
-        <v>0.90300000000000002</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="F20" s="8">
-        <v>0.86499999999999999</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="G20" s="8">
-        <v>0.81299999999999994</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="H20" s="8">
-        <v>0.89500000000000002</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="I20" s="8">
-        <v>0.91900000000000004</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="J20" s="8">
-        <v>0.77100000000000002</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="K20" s="8">
-        <v>0.81100000000000005</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="L20" s="8">
-        <v>0.51600000000000001</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="M20" s="8">
-        <v>0.81200000000000006</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="N20" s="8">
-        <v>0.77600000000000002</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="O20" s="8">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="P20" s="8">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="Q20" s="8"/>
+        <v>0.76</v>
+      </c>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8">
+        <v>0.81499999999999995</v>
+      </c>
       <c r="R20" s="8"/>
       <c r="S20" s="7">
         <v>0.76400000000000001</v>
@@ -7502,7 +7496,7 @@
         <color theme="7" tint="0.39997558519241921"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="76" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
updated coef2 lvl 5 w hampel
</commit_message>
<xml_diff>
--- a/data/Models/ModelResults.xlsx
+++ b/data/Models/ModelResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\OneDrive\Documents\Sandbox\EnvNoiseDetector\data\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{07CBC4EF-469A-4221-ADA7-E18C4BAF1C7A}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="5_{5F5A40D7-0379-4FCB-9829-374C4FE79621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{02E6D408-F3B3-4751-BCE4-62AD87437556}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="876" windowWidth="26940" windowHeight="15732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="0" windowWidth="26940" windowHeight="15732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelResults" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -743,6 +743,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -926,7 +932,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -956,6 +962,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1003,7 +1012,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -5970,13 +5985,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7046,7 +7061,7 @@
       <c r="S22" s="7"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B23">
@@ -7056,7 +7071,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="8">
-        <v>0.80400000000000005</v>
+        <v>0.81</v>
       </c>
       <c r="E23" s="8">
         <v>0.91700000000000004</v>
@@ -7067,7 +7082,9 @@
       <c r="G23" s="8">
         <v>0.79300000000000004</v>
       </c>
-      <c r="H23" s="10"/>
+      <c r="H23" s="10">
+        <v>0.92100000000000004</v>
+      </c>
       <c r="I23" s="8">
         <v>0.94</v>
       </c>
@@ -7075,9 +7092,11 @@
         <v>0.82</v>
       </c>
       <c r="K23" s="8">
-        <v>0.879</v>
-      </c>
-      <c r="L23" s="10"/>
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0.91500000000000004</v>
+      </c>
       <c r="M23" s="8">
         <v>0.876</v>
       </c>
@@ -7090,8 +7109,8 @@
       <c r="P23" s="8">
         <v>0.76500000000000001</v>
       </c>
-      <c r="Q23" s="8" t="s">
-        <v>111</v>
+      <c r="Q23" s="8">
+        <v>0.84899999999999998</v>
       </c>
       <c r="R23" s="8"/>
       <c r="S23" s="7"/>
@@ -7444,27 +7463,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D37" s="3" t="s">
         <v>93</v>
       </c>
@@ -7481,13 +7500,64 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>98</v>
       </c>
     </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D41" s="8">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="E41" s="8">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="F41" s="8">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="G41" s="8">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="H41" s="10"/>
+      <c r="I41" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="J41" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="K41" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="L41" s="10"/>
+      <c r="M41" s="8">
+        <v>0.876</v>
+      </c>
+      <c r="N41" s="8">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="O41" s="8">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="P41" s="8">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="Q41" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D2:S29">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="7" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="top10" dxfId="1" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:Q41">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="90"/>

</xml_diff>